<commit_message>
HC in WIP in data
</commit_message>
<xml_diff>
--- a/metrics_aggregate_dev.xlsx
+++ b/metrics_aggregate_dev.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J166"/>
+  <dimension ref="A1:K166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,15 +475,20 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>HC in WIP</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>fallback_used</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Target UPLH</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Actual UPLH</t>
         </is>
@@ -515,11 +520,14 @@
       <c r="G2" t="n">
         <v>297.5</v>
       </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
         <v>4.49</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>5.5</v>
       </c>
     </row>
@@ -549,11 +557,14 @@
       <c r="G3" t="n">
         <v>237.5</v>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
+      <c r="H3" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
         <v>4.72</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>6.51</v>
       </c>
     </row>
@@ -583,11 +594,14 @@
       <c r="G4" t="n">
         <v>330</v>
       </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
+      <c r="H4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
         <v>4.52</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>4.09</v>
       </c>
     </row>
@@ -617,11 +631,14 @@
       <c r="G5" t="n">
         <v>294.5</v>
       </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
         <v>4.53</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>5.27</v>
       </c>
     </row>
@@ -651,11 +668,14 @@
       <c r="G6" t="n">
         <v>297</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
+      <c r="H6" t="n">
+        <v>10</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
         <v>4.24</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>5.08</v>
       </c>
     </row>
@@ -685,11 +705,14 @@
       <c r="G7" t="n">
         <v>320</v>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="n">
         <v>4.54</v>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>5.2</v>
       </c>
     </row>
@@ -719,11 +742,14 @@
       <c r="G8" t="n">
         <v>275.5</v>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
         <v>4.51</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>5.51</v>
       </c>
     </row>
@@ -753,11 +779,14 @@
       <c r="G9" t="n">
         <v>299.25</v>
       </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
+      <c r="H9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="n">
         <v>4.51</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>4.88</v>
       </c>
     </row>
@@ -787,11 +816,14 @@
       <c r="G10" t="n">
         <v>264.5</v>
       </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
+      <c r="H10" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="n">
         <v>4.44</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>4.74</v>
       </c>
     </row>
@@ -821,11 +853,14 @@
       <c r="G11" t="n">
         <v>355.9</v>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
+      <c r="H11" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
         <v>4.44</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>4.28</v>
       </c>
     </row>
@@ -855,11 +890,14 @@
       <c r="G12" t="n">
         <v>277.5</v>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
         <v>4.33</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>4.08</v>
       </c>
     </row>
@@ -889,11 +927,14 @@
       <c r="G13" t="n">
         <v>382</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
+      <c r="H13" t="n">
+        <v>10</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
         <v>4.38</v>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>3.93</v>
       </c>
     </row>
@@ -923,11 +964,14 @@
       <c r="G14" t="n">
         <v>389.5</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
+      <c r="H14" t="n">
+        <v>10</v>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="n">
         <v>4.44</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>3.71</v>
       </c>
     </row>
@@ -957,11 +1001,14 @@
       <c r="G15" t="n">
         <v>366.5</v>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
+      <c r="H15" t="n">
+        <v>10</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
         <v>4.55</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>3.31</v>
       </c>
     </row>
@@ -991,11 +1038,14 @@
       <c r="G16" t="n">
         <v>375</v>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
+      <c r="H16" t="n">
+        <v>10</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
         <v>4.54</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>3.7</v>
       </c>
     </row>
@@ -1025,11 +1075,14 @@
       <c r="G17" t="n">
         <v>339.5</v>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
+      <c r="H17" t="n">
+        <v>10</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
         <v>4.49</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>3.63</v>
       </c>
     </row>
@@ -1059,11 +1112,14 @@
       <c r="G18" t="n">
         <v>357.25</v>
       </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
+      <c r="H18" t="n">
+        <v>10</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
         <v>4.55</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>3.57</v>
       </c>
     </row>
@@ -1093,11 +1149,14 @@
       <c r="G19" t="n">
         <v>236</v>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
+      <c r="H19" t="n">
+        <v>10</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="n">
         <v>4.56</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>4.93</v>
       </c>
     </row>
@@ -1127,11 +1186,14 @@
       <c r="G20" t="n">
         <v>309.75</v>
       </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="n">
+      <c r="H20" t="n">
+        <v>10</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="n">
         <v>4.56</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>4.2</v>
       </c>
     </row>
@@ -1161,11 +1223,14 @@
       <c r="G21" t="n">
         <v>336.25</v>
       </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
+      <c r="H21" t="n">
+        <v>10</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="n">
         <v>4.5</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>3.99</v>
       </c>
     </row>
@@ -1195,11 +1260,14 @@
       <c r="G22" t="n">
         <v>298.65</v>
       </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
+      <c r="H22" t="n">
+        <v>10</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="n">
         <v>4.61</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>4.74</v>
       </c>
     </row>
@@ -1229,11 +1297,14 @@
       <c r="G23" t="n">
         <v>164.75</v>
       </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="n">
+      <c r="H23" t="n">
+        <v>9</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="n">
         <v>4</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>4.88</v>
       </c>
     </row>
@@ -1263,11 +1334,14 @@
       <c r="G24" t="n">
         <v>272</v>
       </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
+      <c r="H24" t="n">
+        <v>9</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="n">
         <v>4.38</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>4.8</v>
       </c>
     </row>
@@ -1297,11 +1371,14 @@
       <c r="G25" t="n">
         <v>226.5</v>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
+      <c r="H25" t="n">
+        <v>11</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="n">
         <v>4.61</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>4.55</v>
       </c>
     </row>
@@ -1331,11 +1408,14 @@
       <c r="G26" t="n">
         <v>310.75</v>
       </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
+      <c r="H26" t="n">
+        <v>10</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
         <v>4.62</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>4.59</v>
       </c>
     </row>
@@ -1365,11 +1445,14 @@
       <c r="G27" t="n">
         <v>288</v>
       </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="n">
+      <c r="H27" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="n">
         <v>4.69</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>4.34</v>
       </c>
     </row>
@@ -1399,11 +1482,14 @@
       <c r="G28" t="n">
         <v>274.25</v>
       </c>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="n">
+      <c r="H28" t="n">
+        <v>9</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="n">
         <v>4.34</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>5.18</v>
       </c>
     </row>
@@ -1433,11 +1519,14 @@
       <c r="G29" t="n">
         <v>286.75</v>
       </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="n">
+      <c r="H29" t="n">
+        <v>10</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="n">
         <v>4.3</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>5.27</v>
       </c>
     </row>
@@ -1467,11 +1556,14 @@
       <c r="G30" t="n">
         <v>281.25</v>
       </c>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="n">
+      <c r="H30" t="n">
+        <v>9</v>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="n">
         <v>4.53</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>5.27</v>
       </c>
     </row>
@@ -1501,11 +1593,14 @@
       <c r="G31" t="n">
         <v>168.5</v>
       </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="n">
+      <c r="H31" t="n">
+        <v>8</v>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="n">
         <v>4.8</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>5.31</v>
       </c>
     </row>
@@ -1535,11 +1630,14 @@
       <c r="G32" t="n">
         <v>199</v>
       </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="n">
+      <c r="H32" t="n">
+        <v>10</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="n">
         <v>4.77</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>5.37</v>
       </c>
     </row>
@@ -1569,11 +1667,14 @@
       <c r="G33" t="n">
         <v>324.5</v>
       </c>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="n">
+      <c r="H33" t="n">
+        <v>11</v>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="n">
         <v>4.48</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>4.45</v>
       </c>
     </row>
@@ -1603,11 +1704,14 @@
       <c r="G34" t="n">
         <v>233.75</v>
       </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="n">
+      <c r="H34" t="n">
+        <v>10</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="n">
         <v>4.46</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>5.01</v>
       </c>
     </row>
@@ -1637,11 +1741,14 @@
       <c r="G35" t="n">
         <v>389.05</v>
       </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="n">
+      <c r="H35" t="n">
+        <v>11</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="n">
         <v>4.54</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>4.28</v>
       </c>
     </row>
@@ -1671,11 +1778,14 @@
       <c r="G36" t="n">
         <v>403</v>
       </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="n">
+      <c r="H36" t="n">
+        <v>11</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="n">
         <v>4.42</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>4.54</v>
       </c>
     </row>
@@ -1705,11 +1815,14 @@
       <c r="G37" t="n">
         <v>337.5</v>
       </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="n">
+      <c r="H37" t="n">
+        <v>11</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="n">
         <v>4.43</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>3.48</v>
       </c>
     </row>
@@ -1739,11 +1852,14 @@
       <c r="G38" t="n">
         <v>359.1</v>
       </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="n">
+      <c r="H38" t="n">
+        <v>11</v>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="n">
         <v>4.54</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>3.8</v>
       </c>
     </row>
@@ -1773,11 +1889,14 @@
       <c r="G39" t="n">
         <v>349</v>
       </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="n">
+      <c r="H39" t="n">
+        <v>11</v>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="n">
         <v>4.19</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>3.34</v>
       </c>
     </row>
@@ -1807,11 +1926,14 @@
       <c r="G40" t="n">
         <v>379</v>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="n">
+      <c r="H40" t="n">
+        <v>11</v>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="n">
         <v>4.52</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>3.51</v>
       </c>
     </row>
@@ -1841,11 +1963,14 @@
       <c r="G41" t="n">
         <v>322</v>
       </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="n">
+      <c r="H41" t="n">
+        <v>9</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="n">
         <v>4.53</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>3.29</v>
       </c>
     </row>
@@ -1875,11 +2000,14 @@
       <c r="G42" t="n">
         <v>330.5</v>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="n">
+      <c r="H42" t="n">
+        <v>9</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="n">
         <v>4.58</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>4.02</v>
       </c>
     </row>
@@ -1909,11 +2037,14 @@
       <c r="G43" t="n">
         <v>402</v>
       </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="n">
+      <c r="H43" t="n">
+        <v>11</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="n">
         <v>4.38</v>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>3.21</v>
       </c>
     </row>
@@ -1943,11 +2074,14 @@
       <c r="G44" t="n">
         <v>411</v>
       </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="n">
+      <c r="H44" t="n">
+        <v>12</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="n">
         <v>4.3</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>3.61</v>
       </c>
     </row>
@@ -1977,11 +2111,14 @@
       <c r="G45" t="n">
         <v>346</v>
       </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="n">
+      <c r="H45" t="n">
+        <v>13</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="n">
         <v>4.2</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>3.23</v>
       </c>
     </row>
@@ -2011,11 +2148,14 @@
       <c r="G46" t="n">
         <v>447.5</v>
       </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="n">
+      <c r="H46" t="n">
+        <v>14</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="n">
         <v>4.31</v>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>3.43</v>
       </c>
     </row>
@@ -2045,11 +2185,14 @@
       <c r="G47" t="n">
         <v>501</v>
       </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="n">
+      <c r="H47" t="n">
+        <v>14</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="n">
         <v>4.33</v>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>3.67</v>
       </c>
     </row>
@@ -2079,11 +2222,14 @@
       <c r="G48" t="n">
         <v>524.2</v>
       </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="n">
+      <c r="H48" t="n">
+        <v>14</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="n">
         <v>4.35</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>3.61</v>
       </c>
     </row>
@@ -2113,11 +2259,14 @@
       <c r="G49" t="n">
         <v>392</v>
       </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="n">
+      <c r="H49" t="n">
+        <v>13</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="n">
         <v>4.32</v>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>3.88</v>
       </c>
     </row>
@@ -2147,11 +2296,14 @@
       <c r="G50" t="n">
         <v>459.5</v>
       </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="n">
+      <c r="H50" t="n">
+        <v>14</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="n">
         <v>4.23</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>4.17</v>
       </c>
     </row>
@@ -2181,11 +2333,14 @@
       <c r="G51" t="n">
         <v>464.5</v>
       </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="n">
+      <c r="H51" t="n">
+        <v>14</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="n">
         <v>4.29</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>3.94</v>
       </c>
     </row>
@@ -2215,11 +2370,14 @@
       <c r="G52" t="n">
         <v>485</v>
       </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="n">
+      <c r="H52" t="n">
+        <v>14</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="n">
         <v>4.37</v>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>4.35</v>
       </c>
     </row>
@@ -2249,11 +2407,14 @@
       <c r="G53" t="n">
         <v>424</v>
       </c>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="n">
+      <c r="H53" t="n">
+        <v>14</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="n">
         <v>4.38</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>4.19</v>
       </c>
     </row>
@@ -2283,11 +2444,14 @@
       <c r="G54" t="n">
         <v>340.5</v>
       </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="n">
+      <c r="H54" t="n">
+        <v>13</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="n">
         <v>4.36</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>4.15</v>
       </c>
     </row>
@@ -2317,11 +2481,14 @@
       <c r="G55" t="n">
         <v>430.25</v>
       </c>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="n">
+      <c r="H55" t="n">
+        <v>14</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="n">
         <v>4.39</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>4.37</v>
       </c>
     </row>
@@ -2351,11 +2518,14 @@
       <c r="G56" t="n">
         <v>369.25</v>
       </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="n">
+      <c r="H56" t="n">
+        <v>14</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="n">
         <v>4.19</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>3.86</v>
       </c>
     </row>
@@ -2385,11 +2555,14 @@
       <c r="G57" t="n">
         <v>419.5</v>
       </c>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="n">
+      <c r="H57" t="n">
+        <v>13</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="n">
         <v>4.27</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>4.54</v>
       </c>
     </row>
@@ -2419,11 +2592,14 @@
       <c r="G58" t="n">
         <v>409</v>
       </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="n">
+      <c r="H58" t="n">
+        <v>14</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="n">
         <v>4.32</v>
       </c>
-      <c r="J58" t="n">
+      <c r="K58" t="n">
         <v>4.22</v>
       </c>
     </row>
@@ -2453,11 +2629,14 @@
       <c r="G59" t="n">
         <v>380.5</v>
       </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="n">
+      <c r="H59" t="n">
+        <v>13</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="n">
         <v>4</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>4.29</v>
       </c>
     </row>
@@ -2487,11 +2666,14 @@
       <c r="G60" t="n">
         <v>365.75</v>
       </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="n">
+      <c r="H60" t="n">
+        <v>13</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="n">
         <v>4</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>4.08</v>
       </c>
     </row>
@@ -2521,11 +2703,14 @@
       <c r="G61" t="n">
         <v>308.75</v>
       </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="n">
+      <c r="H61" t="n">
+        <v>12</v>
+      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="n">
         <v>4.28</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
         <v>4.38</v>
       </c>
     </row>
@@ -2555,11 +2740,14 @@
       <c r="G62" t="n">
         <v>399</v>
       </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="n">
+      <c r="H62" t="n">
+        <v>14</v>
+      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="n">
         <v>4.4</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>4.54</v>
       </c>
     </row>
@@ -2589,11 +2777,14 @@
       <c r="G63" t="n">
         <v>392.5</v>
       </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="n">
+      <c r="H63" t="n">
+        <v>14</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="n">
         <v>4.38</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>4.41</v>
       </c>
     </row>
@@ -2623,11 +2814,14 @@
       <c r="G64" t="n">
         <v>324</v>
       </c>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="n">
+      <c r="H64" t="n">
+        <v>13</v>
+      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="n">
         <v>4.49</v>
       </c>
-      <c r="J64" t="n">
+      <c r="K64" t="n">
         <v>4.74</v>
       </c>
     </row>
@@ -2657,11 +2851,14 @@
       <c r="G65" t="n">
         <v>408.5</v>
       </c>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="n">
+      <c r="H65" t="n">
+        <v>13</v>
+      </c>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="n">
         <v>4.43</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>4.62</v>
       </c>
     </row>
@@ -2691,11 +2888,14 @@
       <c r="G66" t="n">
         <v>252.5</v>
       </c>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="n">
+      <c r="H66" t="n">
+        <v>13</v>
+      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="n">
         <v>4.58</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>4.99</v>
       </c>
     </row>
@@ -2725,11 +2925,14 @@
       <c r="G67" t="n">
         <v>159.4</v>
       </c>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="n">
+      <c r="H67" t="n">
+        <v>13</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="n">
         <v>3.98</v>
       </c>
-      <c r="J67" t="n">
+      <c r="K67" t="n">
         <v>4.23</v>
       </c>
     </row>
@@ -2759,11 +2962,14 @@
       <c r="G68" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="H68" t="inlineStr"/>
-      <c r="I68" t="n">
+      <c r="H68" t="n">
+        <v>4</v>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="n">
         <v>4.57</v>
       </c>
-      <c r="J68" t="n">
+      <c r="K68" t="n">
         <v>4.51</v>
       </c>
     </row>
@@ -2793,11 +2999,14 @@
       <c r="G69" t="n">
         <v>90.40000000000001</v>
       </c>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="n">
+      <c r="H69" t="n">
+        <v>4</v>
+      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="n">
         <v>4.91</v>
       </c>
-      <c r="J69" t="n">
+      <c r="K69" t="n">
         <v>4.2</v>
       </c>
     </row>
@@ -2827,11 +3036,14 @@
       <c r="G70" t="n">
         <v>89.15000000000001</v>
       </c>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="n">
+      <c r="H70" t="n">
+        <v>4</v>
+      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="n">
         <v>3.84</v>
       </c>
-      <c r="J70" t="n">
+      <c r="K70" t="n">
         <v>3.86</v>
       </c>
     </row>
@@ -2861,11 +3073,14 @@
       <c r="G71" t="n">
         <v>79.40000000000001</v>
       </c>
-      <c r="H71" t="inlineStr"/>
-      <c r="I71" t="n">
+      <c r="H71" t="n">
+        <v>4</v>
+      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="n">
         <v>3.07</v>
       </c>
-      <c r="J71" t="n">
+      <c r="K71" t="n">
         <v>4.07</v>
       </c>
     </row>
@@ -2895,11 +3110,14 @@
       <c r="G72" t="n">
         <v>68.73333333333333</v>
       </c>
-      <c r="H72" t="inlineStr"/>
-      <c r="I72" t="n">
+      <c r="H72" t="n">
+        <v>4</v>
+      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="n">
         <v>2.76</v>
       </c>
-      <c r="J72" t="n">
+      <c r="K72" t="n">
         <v>3.87</v>
       </c>
     </row>
@@ -2929,15 +3147,18 @@
       <c r="G73" t="n">
         <v>73.31666666666666</v>
       </c>
-      <c r="H73" t="inlineStr">
+      <c r="H73" t="n">
+        <v>4</v>
+      </c>
+      <c r="I73" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 4-22-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I73" t="n">
+      <c r="J73" t="n">
         <v>3.93</v>
       </c>
-      <c r="J73" t="n">
+      <c r="K73" t="n">
         <v>4.08</v>
       </c>
     </row>
@@ -2967,15 +3188,18 @@
       <c r="G74" t="n">
         <v>93.73333333333333</v>
       </c>
-      <c r="H74" t="inlineStr">
+      <c r="H74" t="n">
+        <v>5</v>
+      </c>
+      <c r="I74" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 5-6-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I74" t="n">
+      <c r="J74" t="n">
         <v>6.53</v>
       </c>
-      <c r="J74" t="n">
+      <c r="K74" t="n">
         <v>4.67</v>
       </c>
     </row>
@@ -3005,15 +3229,18 @@
       <c r="G75" t="n">
         <v>60.86666666666667</v>
       </c>
-      <c r="H75" t="inlineStr">
+      <c r="H75" t="n">
+        <v>4</v>
+      </c>
+      <c r="I75" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 5-13-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I75" t="n">
+      <c r="J75" t="n">
         <v>2.66</v>
       </c>
-      <c r="J75" t="n">
+      <c r="K75" t="n">
         <v>2.99</v>
       </c>
     </row>
@@ -3043,15 +3270,18 @@
       <c r="G76" t="n">
         <v>77.73333333333333</v>
       </c>
-      <c r="H76" t="inlineStr">
+      <c r="H76" t="n">
+        <v>5</v>
+      </c>
+      <c r="I76" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 5-27-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I76" t="n">
+      <c r="J76" t="n">
         <v>4.32</v>
       </c>
-      <c r="J76" t="n">
+      <c r="K76" t="n">
         <v>3.94</v>
       </c>
     </row>
@@ -3081,15 +3311,18 @@
       <c r="G77" t="n">
         <v>91.98333333333333</v>
       </c>
-      <c r="H77" t="inlineStr">
+      <c r="H77" t="n">
+        <v>5</v>
+      </c>
+      <c r="I77" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-3-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I77" t="n">
+      <c r="J77" t="n">
         <v>4.73</v>
       </c>
-      <c r="J77" t="n">
+      <c r="K77" t="n">
         <v>4.12</v>
       </c>
     </row>
@@ -3119,15 +3352,18 @@
       <c r="G78" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="H78" t="inlineStr">
+      <c r="H78" t="n">
+        <v>5</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-10-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I78" t="n">
+      <c r="J78" t="n">
         <v>4.61</v>
       </c>
-      <c r="J78" t="n">
+      <c r="K78" t="n">
         <v>3.88</v>
       </c>
     </row>
@@ -3157,15 +3393,18 @@
       <c r="G79" t="n">
         <v>108.9833333333333</v>
       </c>
-      <c r="H79" t="inlineStr">
+      <c r="H79" t="n">
+        <v>5</v>
+      </c>
+      <c r="I79" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-17-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I79" t="n">
+      <c r="J79" t="n">
         <v>5.2</v>
       </c>
-      <c r="J79" t="n">
+      <c r="K79" t="n">
         <v>4.88</v>
       </c>
     </row>
@@ -3195,15 +3434,18 @@
       <c r="G80" t="n">
         <v>74.23333333333333</v>
       </c>
-      <c r="H80" t="inlineStr">
+      <c r="H80" t="n">
+        <v>4</v>
+      </c>
+      <c r="I80" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-24-24.xlsm</t>
         </is>
       </c>
-      <c r="I80" t="n">
+      <c r="J80" t="n">
         <v>4.02</v>
       </c>
-      <c r="J80" t="n">
+      <c r="K80" t="n">
         <v>4.46</v>
       </c>
     </row>
@@ -3233,15 +3475,18 @@
       <c r="G81" t="n">
         <v>67.81666666666666</v>
       </c>
-      <c r="H81" t="inlineStr">
+      <c r="H81" t="n">
+        <v>4</v>
+      </c>
+      <c r="I81" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 7-1-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I81" t="n">
+      <c r="J81" t="n">
         <v>3.81</v>
       </c>
-      <c r="J81" t="n">
+      <c r="K81" t="n">
         <v>3.95</v>
       </c>
     </row>
@@ -3271,15 +3516,18 @@
       <c r="G82" t="n">
         <v>90.90000000000001</v>
       </c>
-      <c r="H82" t="inlineStr">
+      <c r="H82" t="n">
+        <v>4</v>
+      </c>
+      <c r="I82" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 7-8-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I82" t="n">
+      <c r="J82" t="n">
         <v>5.05</v>
       </c>
-      <c r="J82" t="n">
+      <c r="K82" t="n">
         <v>3.98</v>
       </c>
     </row>
@@ -3309,15 +3557,18 @@
       <c r="G83" t="n">
         <v>86.73333333333333</v>
       </c>
-      <c r="H83" t="inlineStr">
+      <c r="H83" t="n">
+        <v>4</v>
+      </c>
+      <c r="I83" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 7-15-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I83" t="n">
+      <c r="J83" t="n">
         <v>5.16</v>
       </c>
-      <c r="J83" t="n">
+      <c r="K83" t="n">
         <v>4.21</v>
       </c>
     </row>
@@ -3347,15 +3598,18 @@
       <c r="G84" t="n">
         <v>72.15000000000001</v>
       </c>
-      <c r="H84" t="inlineStr">
+      <c r="H84" t="n">
+        <v>4</v>
+      </c>
+      <c r="I84" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 7-22-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I84" t="n">
+      <c r="J84" t="n">
         <v>4.19</v>
       </c>
-      <c r="J84" t="n">
+      <c r="K84" t="n">
         <v>4.53</v>
       </c>
     </row>
@@ -3385,15 +3639,18 @@
       <c r="G85" t="n">
         <v>47.23333333333333</v>
       </c>
-      <c r="H85" t="inlineStr">
+      <c r="H85" t="n">
+        <v>3</v>
+      </c>
+      <c r="I85" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 7-29-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I85" t="n">
+      <c r="J85" t="n">
         <v>2.39</v>
       </c>
-      <c r="J85" t="n">
+      <c r="K85" t="n">
         <v>4.93</v>
       </c>
     </row>
@@ -3423,15 +3680,18 @@
       <c r="G86" t="n">
         <v>60.23333333333333</v>
       </c>
-      <c r="H86" t="inlineStr">
+      <c r="H86" t="n">
+        <v>3</v>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 8-5-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I86" t="n">
+      <c r="J86" t="n">
         <v>3.31</v>
       </c>
-      <c r="J86" t="n">
+      <c r="K86" t="n">
         <v>4.95</v>
       </c>
     </row>
@@ -3461,15 +3721,18 @@
       <c r="G87" t="n">
         <v>59.73333333333333</v>
       </c>
-      <c r="H87" t="inlineStr">
+      <c r="H87" t="n">
+        <v>4</v>
+      </c>
+      <c r="I87" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 8-12-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I87" t="n">
+      <c r="J87" t="n">
         <v>3.03</v>
       </c>
-      <c r="J87" t="n">
+      <c r="K87" t="n">
         <v>4.52</v>
       </c>
     </row>
@@ -3499,15 +3762,18 @@
       <c r="G88" t="n">
         <v>38.73333333333333</v>
       </c>
-      <c r="H88" t="inlineStr">
+      <c r="H88" t="n">
+        <v>4</v>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 8-19-2024.xlsm</t>
         </is>
       </c>
-      <c r="I88" t="n">
+      <c r="J88" t="n">
         <v>1.87</v>
       </c>
-      <c r="J88" t="n">
+      <c r="K88" t="n">
         <v>4.49</v>
       </c>
     </row>
@@ -3537,15 +3803,18 @@
       <c r="G89" t="n">
         <v>46.9</v>
       </c>
-      <c r="H89" t="inlineStr">
+      <c r="H89" t="n">
+        <v>3</v>
+      </c>
+      <c r="I89" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 9-2-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I89" t="n">
+      <c r="J89" t="n">
         <v>2.16</v>
       </c>
-      <c r="J89" t="n">
+      <c r="K89" t="n">
         <v>4.31</v>
       </c>
     </row>
@@ -3575,15 +3844,18 @@
       <c r="G90" t="n">
         <v>26.23333333333333</v>
       </c>
-      <c r="H90" t="inlineStr">
+      <c r="H90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 9-9-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I90" t="n">
+      <c r="J90" t="n">
         <v>1.3</v>
       </c>
-      <c r="J90" t="n">
+      <c r="K90" t="n">
         <v>4.35</v>
       </c>
     </row>
@@ -3613,15 +3885,18 @@
       <c r="G91" t="n">
         <v>53.23333333333333</v>
       </c>
-      <c r="H91" t="inlineStr">
+      <c r="H91" t="n">
+        <v>3</v>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 9-16-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I91" t="n">
+      <c r="J91" t="n">
         <v>2.43</v>
       </c>
-      <c r="J91" t="n">
+      <c r="K91" t="n">
         <v>4.47</v>
       </c>
     </row>
@@ -3651,15 +3926,18 @@
       <c r="G92" t="n">
         <v>54.23333333333333</v>
       </c>
-      <c r="H92" t="inlineStr">
+      <c r="H92" t="n">
+        <v>4</v>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 9-23-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I92" t="n">
+      <c r="J92" t="n">
         <v>2.69</v>
       </c>
-      <c r="J92" t="n">
+      <c r="K92" t="n">
         <v>3.84</v>
       </c>
     </row>
@@ -3689,15 +3967,18 @@
       <c r="G93" t="n">
         <v>39.73333333333333</v>
       </c>
-      <c r="H93" t="inlineStr">
+      <c r="H93" t="n">
+        <v>4</v>
+      </c>
+      <c r="I93" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 9-30-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I93" t="n">
+      <c r="J93" t="n">
         <v>1.98</v>
       </c>
-      <c r="J93" t="n">
+      <c r="K93" t="n">
         <v>4.38</v>
       </c>
     </row>
@@ -3727,15 +4008,18 @@
       <c r="G94" t="n">
         <v>53.73333333333333</v>
       </c>
-      <c r="H94" t="inlineStr">
+      <c r="H94" t="n">
+        <v>4</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 10-7-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I94" t="n">
+      <c r="J94" t="n">
         <v>2.54</v>
       </c>
-      <c r="J94" t="n">
+      <c r="K94" t="n">
         <v>4.28</v>
       </c>
     </row>
@@ -3765,11 +4049,14 @@
       <c r="G95" t="n">
         <v>20.23333333333333</v>
       </c>
-      <c r="H95" t="inlineStr"/>
-      <c r="I95" t="n">
+      <c r="H95" t="n">
+        <v>2</v>
+      </c>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="n">
         <v>1.04</v>
       </c>
-      <c r="J95" t="n">
+      <c r="K95" t="n">
         <v>2.82</v>
       </c>
     </row>
@@ -3799,15 +4086,18 @@
       <c r="G96" t="n">
         <v>66.56666666666666</v>
       </c>
-      <c r="H96" t="inlineStr">
+      <c r="H96" t="n">
+        <v>4</v>
+      </c>
+      <c r="I96" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from week of 10-28-2024 SVT Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I96" t="n">
+      <c r="J96" t="n">
         <v>2.91</v>
       </c>
-      <c r="J96" t="n">
+      <c r="K96" t="n">
         <v>3.79</v>
       </c>
     </row>
@@ -3837,15 +4127,18 @@
       <c r="G97" t="n">
         <v>61.4</v>
       </c>
-      <c r="H97" t="inlineStr">
+      <c r="H97" t="n">
+        <v>4</v>
+      </c>
+      <c r="I97" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 11-4-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I97" t="n">
+      <c r="J97" t="n">
         <v>2.46</v>
       </c>
-      <c r="J97" t="n">
+      <c r="K97" t="n">
         <v>4.3</v>
       </c>
     </row>
@@ -3875,15 +4168,18 @@
       <c r="G98" t="n">
         <v>66.31666666666666</v>
       </c>
-      <c r="H98" t="inlineStr">
+      <c r="H98" t="n">
+        <v>3</v>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 11-11-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I98" t="n">
+      <c r="J98" t="n">
         <v>2.3</v>
       </c>
-      <c r="J98" t="n">
+      <c r="K98" t="n">
         <v>4.16</v>
       </c>
     </row>
@@ -3913,15 +4209,18 @@
       <c r="G99" t="n">
         <v>66.40000000000001</v>
       </c>
-      <c r="H99" t="inlineStr">
+      <c r="H99" t="n">
+        <v>3</v>
+      </c>
+      <c r="I99" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 12-2-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I99" t="n">
+      <c r="J99" t="n">
         <v>2.08</v>
       </c>
-      <c r="J99" t="n">
+      <c r="K99" t="n">
         <v>3.78</v>
       </c>
     </row>
@@ -3951,15 +4250,18 @@
       <c r="G100" t="n">
         <v>23.23333333333333</v>
       </c>
-      <c r="H100" t="inlineStr">
+      <c r="H100" t="n">
+        <v>3</v>
+      </c>
+      <c r="I100" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 12-9-2024 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I100" t="n">
+      <c r="J100" t="n">
         <v>0.76</v>
       </c>
-      <c r="J100" t="n">
+      <c r="K100" t="n">
         <v>3.62</v>
       </c>
     </row>
@@ -3989,15 +4291,18 @@
       <c r="G101" t="n">
         <v>69.65000000000001</v>
       </c>
-      <c r="H101" t="inlineStr">
+      <c r="H101" t="n">
+        <v>4</v>
+      </c>
+      <c r="I101" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 12-30-24 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I101" t="n">
+      <c r="J101" t="n">
         <v>2.56</v>
       </c>
-      <c r="J101" t="n">
+      <c r="K101" t="n">
         <v>3.24</v>
       </c>
     </row>
@@ -4027,15 +4332,18 @@
       <c r="G102" t="n">
         <v>54.06666666666667</v>
       </c>
-      <c r="H102" t="inlineStr">
+      <c r="H102" t="n">
+        <v>3</v>
+      </c>
+      <c r="I102" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 1-6-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I102" t="n">
+      <c r="J102" t="n">
         <v>1.54</v>
       </c>
-      <c r="J102" t="n">
+      <c r="K102" t="n">
         <v>3.33</v>
       </c>
     </row>
@@ -4065,15 +4373,18 @@
       <c r="G103" t="n">
         <v>44.23333333333333</v>
       </c>
-      <c r="H103" t="inlineStr">
+      <c r="H103" t="n">
+        <v>3</v>
+      </c>
+      <c r="I103" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 1-13-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I103" t="n">
+      <c r="J103" t="n">
         <v>1.6</v>
       </c>
-      <c r="J103" t="n">
+      <c r="K103" t="n">
         <v>4.48</v>
       </c>
     </row>
@@ -4103,15 +4414,18 @@
       <c r="G104" t="n">
         <v>58.75</v>
       </c>
-      <c r="H104" t="inlineStr">
+      <c r="H104" t="n">
+        <v>3</v>
+      </c>
+      <c r="I104" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 1-20-25.xlsm</t>
         </is>
       </c>
-      <c r="I104" t="n">
+      <c r="J104" t="n">
         <v>2.08</v>
       </c>
-      <c r="J104" t="n">
+      <c r="K104" t="n">
         <v>4.09</v>
       </c>
     </row>
@@ -4141,15 +4455,18 @@
       <c r="G105" t="n">
         <v>46.73333333333333</v>
       </c>
-      <c r="H105" t="inlineStr">
+      <c r="H105" t="n">
+        <v>4</v>
+      </c>
+      <c r="I105" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 1-27-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I105" t="n">
+      <c r="J105" t="n">
         <v>1.43</v>
       </c>
-      <c r="J105" t="n">
+      <c r="K105" t="n">
         <v>3.79</v>
       </c>
     </row>
@@ -4179,15 +4496,18 @@
       <c r="G106" t="n">
         <v>67.56666666666666</v>
       </c>
-      <c r="H106" t="inlineStr">
+      <c r="H106" t="n">
+        <v>3</v>
+      </c>
+      <c r="I106" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 2-3-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I106" t="n">
+      <c r="J106" t="n">
         <v>1.45</v>
       </c>
-      <c r="J106" t="n">
+      <c r="K106" t="n">
         <v>3.69</v>
       </c>
     </row>
@@ -4217,15 +4537,18 @@
       <c r="G107" t="n">
         <v>72.06666666666666</v>
       </c>
-      <c r="H107" t="inlineStr">
+      <c r="H107" t="n">
+        <v>4</v>
+      </c>
+      <c r="I107" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 2-10-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I107" t="n">
+      <c r="J107" t="n">
         <v>1.62</v>
       </c>
-      <c r="J107" t="n">
+      <c r="K107" t="n">
         <v>4.05</v>
       </c>
     </row>
@@ -4255,15 +4578,18 @@
       <c r="G108" t="n">
         <v>60.06666666666667</v>
       </c>
-      <c r="H108" t="inlineStr">
+      <c r="H108" t="n">
+        <v>4</v>
+      </c>
+      <c r="I108" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 2-17-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I108" t="n">
+      <c r="J108" t="n">
         <v>1.22</v>
       </c>
-      <c r="J108" t="n">
+      <c r="K108" t="n">
         <v>3.1</v>
       </c>
     </row>
@@ -4293,15 +4619,18 @@
       <c r="G109" t="n">
         <v>56.75</v>
       </c>
-      <c r="H109" t="inlineStr">
+      <c r="H109" t="n">
+        <v>3</v>
+      </c>
+      <c r="I109" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 2-24-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I109" t="n">
+      <c r="J109" t="n">
         <v>1.54</v>
       </c>
-      <c r="J109" t="n">
+      <c r="K109" t="n">
         <v>3.7</v>
       </c>
     </row>
@@ -4331,15 +4660,18 @@
       <c r="G110" t="n">
         <v>32.73333333333333</v>
       </c>
-      <c r="H110" t="inlineStr">
+      <c r="H110" t="n">
+        <v>4</v>
+      </c>
+      <c r="I110" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 3-3-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I110" t="n">
+      <c r="J110" t="n">
         <v>0.93</v>
       </c>
-      <c r="J110" t="n">
+      <c r="K110" t="n">
         <v>3.94</v>
       </c>
     </row>
@@ -4369,15 +4701,18 @@
       <c r="G111" t="n">
         <v>23.4</v>
       </c>
-      <c r="H111" t="inlineStr">
+      <c r="H111" t="n">
+        <v>4</v>
+      </c>
+      <c r="I111" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 3-10-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I111" t="n">
+      <c r="J111" t="n">
         <v>0.45</v>
       </c>
-      <c r="J111" t="n">
+      <c r="K111" t="n">
         <v>4.1</v>
       </c>
     </row>
@@ -4407,15 +4742,18 @@
       <c r="G112" t="n">
         <v>28.06666666666667</v>
       </c>
-      <c r="H112" t="inlineStr">
+      <c r="H112" t="n">
+        <v>2</v>
+      </c>
+      <c r="I112" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 3-17-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I112" t="n">
+      <c r="J112" t="n">
         <v>0.62</v>
       </c>
-      <c r="J112" t="n">
+      <c r="K112" t="n">
         <v>4.6</v>
       </c>
     </row>
@@ -4445,15 +4783,18 @@
       <c r="G113" t="n">
         <v>8.733333333333333</v>
       </c>
-      <c r="H113" t="inlineStr">
+      <c r="H113" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 3-24-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I113" t="n">
+      <c r="J113" t="n">
         <v>0.28</v>
       </c>
-      <c r="J113" t="n">
+      <c r="K113" t="n">
         <v>3.44</v>
       </c>
     </row>
@@ -4483,15 +4824,18 @@
       <c r="G114" t="n">
         <v>12.23333333333333</v>
       </c>
-      <c r="H114" t="inlineStr">
+      <c r="H114" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 3-30-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I114" t="n">
+      <c r="J114" t="n">
         <v>0.43</v>
       </c>
-      <c r="J114" t="n">
+      <c r="K114" t="n">
         <v>6.21</v>
       </c>
     </row>
@@ -4521,15 +4865,18 @@
       <c r="G115" t="n">
         <v>11.73333333333333</v>
       </c>
-      <c r="H115" t="inlineStr">
+      <c r="H115" t="n">
+        <v>1</v>
+      </c>
+      <c r="I115" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 4-14-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I115" t="n">
+      <c r="J115" t="n">
         <v>0.33</v>
       </c>
-      <c r="J115" t="n">
+      <c r="K115" t="n">
         <v>4.26</v>
       </c>
     </row>
@@ -4559,15 +4906,18 @@
       <c r="G116" t="n">
         <v>8.233333333333333</v>
       </c>
-      <c r="H116" t="inlineStr">
+      <c r="H116" t="n">
+        <v>1</v>
+      </c>
+      <c r="I116" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 4-21-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I116" t="n">
+      <c r="J116" t="n">
         <v>0.15</v>
       </c>
-      <c r="J116" t="n">
+      <c r="K116" t="n">
         <v>5.34</v>
       </c>
     </row>
@@ -4597,15 +4947,18 @@
       <c r="G117" t="n">
         <v>19.23333333333333</v>
       </c>
-      <c r="H117" t="inlineStr">
+      <c r="H117" t="n">
+        <v>2</v>
+      </c>
+      <c r="I117" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 4-28-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I117" t="n">
+      <c r="J117" t="n">
         <v>0.49</v>
       </c>
-      <c r="J117" t="n">
+      <c r="K117" t="n">
         <v>3.95</v>
       </c>
     </row>
@@ -4635,15 +4988,18 @@
       <c r="G118" t="n">
         <v>18.23333333333333</v>
       </c>
-      <c r="H118" t="inlineStr">
+      <c r="H118" t="n">
+        <v>1</v>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 5-19-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I118" t="n">
+      <c r="J118" t="n">
         <v>0.4</v>
       </c>
-      <c r="J118" t="n">
+      <c r="K118" t="n">
         <v>3.02</v>
       </c>
     </row>
@@ -4673,15 +5029,18 @@
       <c r="G119" t="n">
         <v>20.23333333333333</v>
       </c>
-      <c r="H119" t="inlineStr">
+      <c r="H119" t="n">
+        <v>1</v>
+      </c>
+      <c r="I119" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 5-26-2025 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I119" t="n">
+      <c r="J119" t="n">
         <v>0.41</v>
       </c>
-      <c r="J119" t="n">
+      <c r="K119" t="n">
         <v>3.31</v>
       </c>
     </row>
@@ -4711,15 +5070,18 @@
       <c r="G120" t="n">
         <v>6.233333333333333</v>
       </c>
-      <c r="H120" t="inlineStr">
+      <c r="H120" t="n">
+        <v>1</v>
+      </c>
+      <c r="I120" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-9-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I120" t="n">
+      <c r="J120" t="n">
         <v>0.17</v>
       </c>
-      <c r="J120" t="n">
+      <c r="K120" t="n">
         <v>3.37</v>
       </c>
     </row>
@@ -4749,15 +5111,18 @@
       <c r="G121" t="n">
         <v>17.23333333333333</v>
       </c>
-      <c r="H121" t="inlineStr">
+      <c r="H121" t="n">
+        <v>1</v>
+      </c>
+      <c r="I121" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-16-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I121" t="n">
+      <c r="J121" t="n">
         <v>0.38</v>
       </c>
-      <c r="J121" t="n">
+      <c r="K121" t="n">
         <v>4.06</v>
       </c>
     </row>
@@ -4787,15 +5152,18 @@
       <c r="G122" t="n">
         <v>24.23333333333333</v>
       </c>
-      <c r="H122" t="inlineStr">
+      <c r="H122" t="n">
+        <v>1</v>
+      </c>
+      <c r="I122" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-23-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I122" t="n">
+      <c r="J122" t="n">
         <v>0.58</v>
       </c>
-      <c r="J122" t="n">
+      <c r="K122" t="n">
         <v>3.59</v>
       </c>
     </row>
@@ -4825,15 +5193,18 @@
       <c r="G123" t="n">
         <v>22.23333333333333</v>
       </c>
-      <c r="H123" t="inlineStr">
+      <c r="H123" t="n">
+        <v>1</v>
+      </c>
+      <c r="I123" t="inlineStr">
         <is>
           <t>Next Weeks Hours!I from Week of 6-30-25 Heijunka.xlsm</t>
         </is>
       </c>
-      <c r="I123" t="n">
+      <c r="J123" t="n">
         <v>0.47</v>
       </c>
-      <c r="J123" t="n">
+      <c r="K123" t="n">
         <v>3.91</v>
       </c>
     </row>
@@ -4863,11 +5234,14 @@
       <c r="G124" t="n">
         <v>24.23333333333333</v>
       </c>
-      <c r="H124" t="inlineStr"/>
-      <c r="I124" t="n">
+      <c r="H124" t="n">
+        <v>1</v>
+      </c>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="n">
         <v>0.62</v>
       </c>
-      <c r="J124" t="n">
+      <c r="K124" t="n">
         <v>2.56</v>
       </c>
     </row>
@@ -4897,11 +5271,14 @@
       <c r="G125" t="n">
         <v>53.58333333333334</v>
       </c>
-      <c r="H125" t="inlineStr"/>
-      <c r="I125" t="n">
+      <c r="H125" t="n">
+        <v>2</v>
+      </c>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="n">
         <v>6.9</v>
       </c>
-      <c r="J125" t="n">
+      <c r="K125" t="n">
         <v>4.85</v>
       </c>
     </row>
@@ -4931,11 +5308,14 @@
       <c r="G126" t="n">
         <v>56.24999999999999</v>
       </c>
-      <c r="H126" t="inlineStr"/>
-      <c r="I126" t="n">
+      <c r="H126" t="n">
+        <v>2</v>
+      </c>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="n">
         <v>7.12</v>
       </c>
-      <c r="J126" t="n">
+      <c r="K126" t="n">
         <v>4.6</v>
       </c>
     </row>
@@ -4965,11 +5345,14 @@
       <c r="G127" t="n">
         <v>46.43333333333334</v>
       </c>
-      <c r="H127" t="inlineStr"/>
-      <c r="I127" t="n">
+      <c r="H127" t="n">
+        <v>3</v>
+      </c>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="n">
         <v>2.62</v>
       </c>
-      <c r="J127" t="n">
+      <c r="K127" t="n">
         <v>4.03</v>
       </c>
     </row>
@@ -4999,11 +5382,14 @@
       <c r="G128" t="n">
         <v>59.16666666666666</v>
       </c>
-      <c r="H128" t="inlineStr"/>
-      <c r="I128" t="n">
+      <c r="H128" t="n">
+        <v>4</v>
+      </c>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="n">
         <v>5.88</v>
       </c>
-      <c r="J128" t="n">
+      <c r="K128" t="n">
         <v>4.26</v>
       </c>
     </row>
@@ -5033,11 +5419,14 @@
       <c r="G129" t="n">
         <v>63.83333333333334</v>
       </c>
-      <c r="H129" t="inlineStr"/>
-      <c r="I129" t="n">
+      <c r="H129" t="n">
+        <v>4</v>
+      </c>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" t="n">
         <v>2.42</v>
       </c>
-      <c r="J129" t="n">
+      <c r="K129" t="n">
         <v>4.89</v>
       </c>
     </row>
@@ -5067,11 +5456,14 @@
       <c r="G130" t="n">
         <v>59.61666666666667</v>
       </c>
-      <c r="H130" t="inlineStr"/>
-      <c r="I130" t="n">
+      <c r="H130" t="n">
+        <v>4</v>
+      </c>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" t="n">
         <v>5.06</v>
       </c>
-      <c r="J130" t="n">
+      <c r="K130" t="n">
         <v>7.21</v>
       </c>
     </row>
@@ -5101,11 +5493,14 @@
       <c r="G131" t="n">
         <v>60</v>
       </c>
-      <c r="H131" t="inlineStr"/>
-      <c r="I131" t="n">
+      <c r="H131" t="n">
+        <v>4</v>
+      </c>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" t="n">
         <v>7.41</v>
       </c>
-      <c r="J131" t="n">
+      <c r="K131" t="n">
         <v>4.77</v>
       </c>
     </row>
@@ -5135,11 +5530,14 @@
       <c r="G132" t="n">
         <v>59.33333333333334</v>
       </c>
-      <c r="H132" t="inlineStr"/>
-      <c r="I132" t="n">
+      <c r="H132" t="n">
+        <v>4</v>
+      </c>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" t="n">
         <v>6.09</v>
       </c>
-      <c r="J132" t="n">
+      <c r="K132" t="n">
         <v>5.33</v>
       </c>
     </row>
@@ -5169,11 +5567,14 @@
       <c r="G133" t="n">
         <v>59.41666666666667</v>
       </c>
-      <c r="H133" t="inlineStr"/>
-      <c r="I133" t="n">
+      <c r="H133" t="n">
+        <v>4</v>
+      </c>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" t="n">
         <v>2.27</v>
       </c>
-      <c r="J133" t="n">
+      <c r="K133" t="n">
         <v>4.22</v>
       </c>
     </row>
@@ -5203,11 +5604,14 @@
       <c r="G134" t="n">
         <v>74.99999999999999</v>
       </c>
-      <c r="H134" t="inlineStr"/>
-      <c r="I134" t="n">
+      <c r="H134" t="n">
+        <v>3</v>
+      </c>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" t="n">
         <v>8.44</v>
       </c>
-      <c r="J134" t="n">
+      <c r="K134" t="n">
         <v>4.29</v>
       </c>
     </row>
@@ -5237,11 +5641,14 @@
       <c r="G135" t="n">
         <v>75.41666666666667</v>
       </c>
-      <c r="H135" t="inlineStr"/>
-      <c r="I135" t="n">
+      <c r="H135" t="n">
+        <v>3</v>
+      </c>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" t="n">
         <v>8</v>
       </c>
-      <c r="J135" t="n">
+      <c r="K135" t="n">
         <v>4.08</v>
       </c>
     </row>
@@ -5271,11 +5678,14 @@
       <c r="G136" t="n">
         <v>55.16666666666667</v>
       </c>
-      <c r="H136" t="inlineStr"/>
-      <c r="I136" t="n">
+      <c r="H136" t="n">
+        <v>3</v>
+      </c>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" t="n">
         <v>7.07</v>
       </c>
-      <c r="J136" t="n">
+      <c r="K136" t="n">
         <v>4.37</v>
       </c>
     </row>
@@ -5305,11 +5715,14 @@
       <c r="G137" t="n">
         <v>39</v>
       </c>
-      <c r="H137" t="inlineStr"/>
-      <c r="I137" t="n">
+      <c r="H137" t="n">
+        <v>4</v>
+      </c>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" t="n">
         <v>8.93</v>
       </c>
-      <c r="J137" t="n">
+      <c r="K137" t="n">
         <v>5.97</v>
       </c>
     </row>
@@ -5339,11 +5752,14 @@
       <c r="G138" t="n">
         <v>67.25</v>
       </c>
-      <c r="H138" t="inlineStr"/>
-      <c r="I138" t="n">
+      <c r="H138" t="n">
+        <v>4</v>
+      </c>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" t="n">
         <v>7.89</v>
       </c>
-      <c r="J138" t="n">
+      <c r="K138" t="n">
         <v>5.52</v>
       </c>
     </row>
@@ -5373,11 +5789,14 @@
       <c r="G139" t="n">
         <v>82.25000000000001</v>
       </c>
-      <c r="H139" t="inlineStr"/>
-      <c r="I139" t="n">
+      <c r="H139" t="n">
+        <v>4</v>
+      </c>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" t="n">
         <v>7.19</v>
       </c>
-      <c r="J139" t="n">
+      <c r="K139" t="n">
         <v>3.51</v>
       </c>
     </row>
@@ -5407,11 +5826,14 @@
       <c r="G140" t="n">
         <v>67.16666666666667</v>
       </c>
-      <c r="H140" t="inlineStr"/>
-      <c r="I140" t="n">
+      <c r="H140" t="n">
+        <v>4</v>
+      </c>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" t="n">
         <v>6.04</v>
       </c>
-      <c r="J140" t="n">
+      <c r="K140" t="n">
         <v>3.62</v>
       </c>
     </row>
@@ -5441,11 +5863,14 @@
       <c r="G141" t="n">
         <v>54.58333333333334</v>
       </c>
-      <c r="H141" t="inlineStr"/>
-      <c r="I141" t="n">
+      <c r="H141" t="n">
+        <v>3</v>
+      </c>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" t="n">
         <v>6.27</v>
       </c>
-      <c r="J141" t="n">
+      <c r="K141" t="n">
         <v>4.27</v>
       </c>
     </row>
@@ -5475,11 +5900,14 @@
       <c r="G142" t="n">
         <v>57.65000000000001</v>
       </c>
-      <c r="H142" t="inlineStr"/>
-      <c r="I142" t="n">
+      <c r="H142" t="n">
+        <v>5</v>
+      </c>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" t="n">
         <v>8.130000000000001</v>
       </c>
-      <c r="J142" t="n">
+      <c r="K142" t="n">
         <v>5.03</v>
       </c>
     </row>
@@ -5509,11 +5937,14 @@
       <c r="G143" t="n">
         <v>43.58333333333334</v>
       </c>
-      <c r="H143" t="inlineStr"/>
-      <c r="I143" t="n">
+      <c r="H143" t="n">
+        <v>4</v>
+      </c>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" t="n">
         <v>13.22</v>
       </c>
-      <c r="J143" t="n">
+      <c r="K143" t="n">
         <v>7.04</v>
       </c>
     </row>
@@ -5543,11 +5974,14 @@
       <c r="G144" t="n">
         <v>67.08333333333333</v>
       </c>
-      <c r="H144" t="inlineStr"/>
-      <c r="I144" t="n">
+      <c r="H144" t="n">
+        <v>4</v>
+      </c>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" t="n">
         <v>17.06</v>
       </c>
-      <c r="J144" t="n">
+      <c r="K144" t="n">
         <v>9.869999999999999</v>
       </c>
     </row>
@@ -5572,17 +6006,20 @@
         <v>245.5</v>
       </c>
       <c r="F145" t="n">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G145" t="n">
-        <v>32.5</v>
-      </c>
-      <c r="H145" t="inlineStr"/>
-      <c r="I145" t="n">
+        <v>32.66666666666666</v>
+      </c>
+      <c r="H145" t="n">
+        <v>3</v>
+      </c>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" t="n">
         <v>7.44</v>
       </c>
-      <c r="J145" t="n">
-        <v>6.68</v>
+      <c r="K145" t="n">
+        <v>6.67</v>
       </c>
     </row>
     <row r="146">
@@ -5611,11 +6048,14 @@
       <c r="G146" t="n">
         <v>130.75</v>
       </c>
-      <c r="H146" t="inlineStr"/>
-      <c r="I146" t="n">
+      <c r="H146" t="n">
+        <v>11</v>
+      </c>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" t="n">
         <v>3.5</v>
       </c>
-      <c r="J146" t="n">
+      <c r="K146" t="n">
         <v>5.24</v>
       </c>
     </row>
@@ -5645,11 +6085,14 @@
       <c r="G147" t="n">
         <v>133.8333333333333</v>
       </c>
-      <c r="H147" t="inlineStr"/>
-      <c r="I147" t="n">
+      <c r="H147" t="n">
+        <v>12</v>
+      </c>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" t="n">
         <v>3.18</v>
       </c>
-      <c r="J147" t="n">
+      <c r="K147" t="n">
         <v>5.02</v>
       </c>
     </row>
@@ -5679,11 +6122,14 @@
       <c r="G148" t="n">
         <v>112.2166666666667</v>
       </c>
-      <c r="H148" t="inlineStr"/>
-      <c r="I148" t="n">
+      <c r="H148" t="n">
+        <v>12</v>
+      </c>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" t="n">
         <v>2.9</v>
       </c>
-      <c r="J148" t="n">
+      <c r="K148" t="n">
         <v>5.84</v>
       </c>
     </row>
@@ -5713,11 +6159,14 @@
       <c r="G149" t="n">
         <v>120.75</v>
       </c>
-      <c r="H149" t="inlineStr"/>
-      <c r="I149" t="n">
+      <c r="H149" t="n">
+        <v>12</v>
+      </c>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" t="n">
         <v>3.58</v>
       </c>
-      <c r="J149" t="n">
+      <c r="K149" t="n">
         <v>6.62</v>
       </c>
     </row>
@@ -5747,11 +6196,14 @@
       <c r="G150" t="n">
         <v>144.0833333333333</v>
       </c>
-      <c r="H150" t="inlineStr"/>
-      <c r="I150" t="n">
+      <c r="H150" t="n">
+        <v>12</v>
+      </c>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="n">
         <v>3.79</v>
       </c>
-      <c r="J150" t="n">
+      <c r="K150" t="n">
         <v>5.95</v>
       </c>
     </row>
@@ -5781,11 +6233,14 @@
       <c r="G151" t="n">
         <v>115.6666666666667</v>
       </c>
-      <c r="H151" t="inlineStr"/>
-      <c r="I151" t="n">
+      <c r="H151" t="n">
+        <v>11</v>
+      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="n">
         <v>3.62</v>
       </c>
-      <c r="J151" t="n">
+      <c r="K151" t="n">
         <v>6.81</v>
       </c>
     </row>
@@ -5815,11 +6270,14 @@
       <c r="G152" t="n">
         <v>80.33333333333333</v>
       </c>
-      <c r="H152" t="inlineStr"/>
-      <c r="I152" t="n">
+      <c r="H152" t="n">
+        <v>12</v>
+      </c>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" t="n">
         <v>4.2</v>
       </c>
-      <c r="J152" t="n">
+      <c r="K152" t="n">
         <v>8.74</v>
       </c>
     </row>
@@ -5849,11 +6307,14 @@
       <c r="G153" t="n">
         <v>107</v>
       </c>
-      <c r="H153" t="inlineStr"/>
-      <c r="I153" t="n">
+      <c r="H153" t="n">
+        <v>12</v>
+      </c>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" t="n">
         <v>3.79</v>
       </c>
-      <c r="J153" t="n">
+      <c r="K153" t="n">
         <v>6.9</v>
       </c>
     </row>
@@ -5883,11 +6344,14 @@
       <c r="G154" t="n">
         <v>111.8333333333333</v>
       </c>
-      <c r="H154" t="inlineStr"/>
-      <c r="I154" t="n">
+      <c r="H154" t="n">
+        <v>11</v>
+      </c>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="n">
         <v>3.63</v>
       </c>
-      <c r="J154" t="n">
+      <c r="K154" t="n">
         <v>6.11</v>
       </c>
     </row>
@@ -5917,11 +6381,14 @@
       <c r="G155" t="n">
         <v>108.1666666666667</v>
       </c>
-      <c r="H155" t="inlineStr"/>
-      <c r="I155" t="n">
+      <c r="H155" t="n">
+        <v>9</v>
+      </c>
+      <c r="I155" t="inlineStr"/>
+      <c r="J155" t="n">
         <v>3.65</v>
       </c>
-      <c r="J155" t="n">
+      <c r="K155" t="n">
         <v>7.45</v>
       </c>
     </row>
@@ -5951,11 +6418,14 @@
       <c r="G156" t="n">
         <v>126.5</v>
       </c>
-      <c r="H156" t="inlineStr"/>
-      <c r="I156" t="n">
+      <c r="H156" t="n">
+        <v>12</v>
+      </c>
+      <c r="I156" t="inlineStr"/>
+      <c r="J156" t="n">
         <v>3.64</v>
       </c>
-      <c r="J156" t="n">
+      <c r="K156" t="n">
         <v>6.27</v>
       </c>
     </row>
@@ -5985,11 +6455,14 @@
       <c r="G157" t="n">
         <v>89.33333333333333</v>
       </c>
-      <c r="H157" t="inlineStr"/>
-      <c r="I157" t="n">
+      <c r="H157" t="n">
+        <v>11</v>
+      </c>
+      <c r="I157" t="inlineStr"/>
+      <c r="J157" t="n">
         <v>3.44</v>
       </c>
-      <c r="J157" t="n">
+      <c r="K157" t="n">
         <v>6.87</v>
       </c>
     </row>
@@ -6019,11 +6492,14 @@
       <c r="G158" t="n">
         <v>88.25</v>
       </c>
-      <c r="H158" t="inlineStr"/>
-      <c r="I158" t="n">
+      <c r="H158" t="n">
+        <v>10</v>
+      </c>
+      <c r="I158" t="inlineStr"/>
+      <c r="J158" t="n">
         <v>3.57</v>
       </c>
-      <c r="J158" t="n">
+      <c r="K158" t="n">
         <v>9.970000000000001</v>
       </c>
     </row>
@@ -6053,11 +6529,14 @@
       <c r="G159" t="n">
         <v>104.1666666666667</v>
       </c>
-      <c r="H159" t="inlineStr"/>
-      <c r="I159" t="n">
+      <c r="H159" t="n">
+        <v>10</v>
+      </c>
+      <c r="I159" t="inlineStr"/>
+      <c r="J159" t="n">
         <v>3.72</v>
       </c>
-      <c r="J159" t="n">
+      <c r="K159" t="n">
         <v>6.15</v>
       </c>
     </row>
@@ -6087,11 +6566,14 @@
       <c r="G160" t="n">
         <v>104.6666666666667</v>
       </c>
-      <c r="H160" t="inlineStr"/>
-      <c r="I160" t="n">
+      <c r="H160" t="n">
+        <v>11</v>
+      </c>
+      <c r="I160" t="inlineStr"/>
+      <c r="J160" t="n">
         <v>4.39</v>
       </c>
-      <c r="J160" t="n">
+      <c r="K160" t="n">
         <v>6.59</v>
       </c>
     </row>
@@ -6121,11 +6603,14 @@
       <c r="G161" t="n">
         <v>114.5</v>
       </c>
-      <c r="H161" t="inlineStr"/>
-      <c r="I161" t="n">
+      <c r="H161" t="n">
+        <v>11</v>
+      </c>
+      <c r="I161" t="inlineStr"/>
+      <c r="J161" t="n">
         <v>3.62</v>
       </c>
-      <c r="J161" t="n">
+      <c r="K161" t="n">
         <v>5.75</v>
       </c>
     </row>
@@ -6155,11 +6640,14 @@
       <c r="G162" t="n">
         <v>94.75</v>
       </c>
-      <c r="H162" t="inlineStr"/>
-      <c r="I162" t="n">
+      <c r="H162" t="n">
+        <v>11</v>
+      </c>
+      <c r="I162" t="inlineStr"/>
+      <c r="J162" t="n">
         <v>3.8</v>
       </c>
-      <c r="J162" t="n">
+      <c r="K162" t="n">
         <v>7.12</v>
       </c>
     </row>
@@ -6189,11 +6677,14 @@
       <c r="G163" t="n">
         <v>88.66666666666666</v>
       </c>
-      <c r="H163" t="inlineStr"/>
-      <c r="I163" t="n">
+      <c r="H163" t="n">
+        <v>12</v>
+      </c>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" t="n">
         <v>2.83</v>
       </c>
-      <c r="J163" t="n">
+      <c r="K163" t="n">
         <v>6</v>
       </c>
     </row>
@@ -6223,11 +6714,14 @@
       <c r="G164" t="n">
         <v>115.0833333333333</v>
       </c>
-      <c r="H164" t="inlineStr"/>
-      <c r="I164" t="n">
+      <c r="H164" t="n">
+        <v>11</v>
+      </c>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" t="n">
         <v>3.23</v>
       </c>
-      <c r="J164" t="n">
+      <c r="K164" t="n">
         <v>8.359999999999999</v>
       </c>
     </row>
@@ -6257,11 +6751,14 @@
       <c r="G165" t="n">
         <v>96.16666666666667</v>
       </c>
-      <c r="H165" t="inlineStr"/>
-      <c r="I165" t="n">
+      <c r="H165" t="n">
+        <v>12</v>
+      </c>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" t="n">
         <v>3.94</v>
       </c>
-      <c r="J165" t="n">
+      <c r="K165" t="n">
         <v>6.88</v>
       </c>
     </row>
@@ -6286,17 +6783,20 @@
         <v>245.5</v>
       </c>
       <c r="F166" t="n">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G166" t="n">
         <v>31</v>
       </c>
-      <c r="H166" t="inlineStr"/>
-      <c r="I166" t="n">
+      <c r="H166" t="n">
+        <v>10</v>
+      </c>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" t="n">
         <v>1.95</v>
       </c>
-      <c r="J166" t="n">
-        <v>7</v>
+      <c r="K166" t="n">
+        <v>7.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ECT and CRDN are good
</commit_message>
<xml_diff>
--- a/metrics_aggregate_dev.xlsx
+++ b/metrics_aggregate_dev.xlsx
@@ -4515,19 +4515,19 @@
         <v>190</v>
       </c>
       <c r="E61" t="n">
-        <v>84.58333333333333</v>
+        <v>99.08333333333333</v>
       </c>
       <c r="F61" t="n">
-        <v>259</v>
+        <v>326</v>
       </c>
       <c r="G61" t="n">
-        <v>227</v>
+        <v>292</v>
       </c>
       <c r="H61" t="n">
-        <v>1.36</v>
+        <v>1.72</v>
       </c>
       <c r="I61" t="n">
-        <v>2.68</v>
+        <v>2.95</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
@@ -4535,34 +4535,34 @@
         <v>7</v>
       </c>
       <c r="M61" t="n">
-        <v>2.6</v>
+        <v>3.05</v>
       </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr">
         <is>
-          <t>{"Ciara": {"actual": 2.0, "available": 0.0}, "Lidiane": {"actual": 11.42, "available": 30.0}, "Kirsty": {"actual": 17.0, "available": 30.0}, "Michelle": {"actual": 10.92, "available": 30.0}, "Alison": {"actual": 0.0, "available": 0.0}, "Louise": {"actual": 0.0, "available": 0.0}, "Grainne": {"actual": 5.5, "available": 16.0}, "Ana": {"actual": 7.75, "available": 24.0}, "Mary": {"actual": 13.0, "available": 30.0}}</t>
+          <t>{"Ciara": {"actual": 2.0, "available": 0.0}, "Lidiane": {"actual": 11.42, "available": 30.0}, "Kirsty": {"actual": 17.0, "available": 30.0}, "Michelle": {"actual": 16.75, "available": 30.0}, "Alison": {"actual": 0.0, "available": 0.0}, "Louise": {"actual": 0.0, "available": 0.0}, "Grainne": {"actual": 7.0, "available": 16.0}, "Ana": {"actual": 11.75, "available": 24.0}, "Mary": {"actual": 16.17, "available": 30.0}}</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>{"Ana": {"output": 34.0, "target": 39.0}, "Ciara": {"output": 66.0, "target": 21.0}, "Grainne": {"output": 16.0, "target": 33.0}, "Kirsty": {"output": 20.0, "target": 43.0}, "Lidiane": {"output": 35.0, "target": 37.0}, "Mary": {"output": 36.0, "target": 44.0}, "Michelle": {"output": 20.0, "target": 42.0}}</t>
+          <t>{"Ana": {"output": 58.0, "target": 60.0}, "Ciara": {"output": 66.0, "target": 21.0}, "Grainne": {"output": 27.0, "target": 48.0}, "Kirsty": {"output": 24.0, "target": 43.0}, "Lidiane": {"output": 35.0, "target": 37.0}, "Mary": {"output": 44.0, "target": 50.0}, "Michelle": {"output": 38.0, "target": 67.0}}</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>{"Closures": {"output": 25.0, "target": 45.0}, "GFE": {"output": 13.0, "target": 25.0}, "Inbox": {"output": 62.0, "target": 18.0}, "New Information": {"output": 43.0, "target": 49.0}, "Other": {"output": 0.0, "target": 0.0}, "ReRD (Reassess RD)": {"output": 15.0, "target": 13.0}, "Regulatory Reports (RR's)": {"output": 14.0, "target": 21.0}, "SR's (Staging Records)": {"output": 28.0, "target": 59.0}, "SR/RD WP2 - Pending RD's": {"output": 27.0, "target": 29.0}}</t>
+          <t>{"Closures": {"output": 39.0, "target": 68.0}, "GFE": {"output": 24.0, "target": 40.0}, "Inbox": {"output": 62.0, "target": 18.0}, "New Information": {"output": 74.0, "target": 74.0}, "Other": {"output": 0.0, "target": 0.0}, "ReRD (Reassess RD)": {"output": 15.0, "target": 13.0}, "Regulatory Reports (RR's)": {"output": 19.0, "target": 25.0}, "SR's (Staging Records)": {"output": 32.0, "target": 59.0}, "SR/RD WP2 - Pending RD's": {"output": 27.0, "target": 29.0}}</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>{"Closures": 10.33, "GFE": 2.5, "Inbox": 1.5, "New Information": 9.58, "ReRD (Reassess RD)": 1.92, "Regulatory Reports (RR's)": 8.67, "SR's (Staging Records)": 23.33, "SR/RD WP2 - Pending RD's": 9.75}</t>
+          <t>{"Closures": 15.67, "GFE": 4.0, "Inbox": 1.5, "New Information": 15.75, "ReRD (Reassess RD)": 1.92, "Regulatory Reports (RR's)": 10.17, "SR's (Staging Records)": 23.33, "SR/RD WP2 - Pending RD's": 9.75}</t>
         </is>
       </c>
       <c r="S61" t="n">
         <v>90</v>
       </c>
       <c r="T61" t="n">
-        <v>67.58333333333333</v>
+        <v>82.08333333333333</v>
       </c>
       <c r="U61" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
TCT Clin is good
</commit_message>
<xml_diff>
--- a/metrics_aggregate_dev.xlsx
+++ b/metrics_aggregate_dev.xlsx
@@ -23583,19 +23583,19 @@
         <v>43.5</v>
       </c>
       <c r="E363" t="n">
-        <v>23.33333333333334</v>
+        <v>26.33333333333334</v>
       </c>
       <c r="F363" t="n">
-        <v>139.5</v>
+        <v>155.5</v>
       </c>
       <c r="G363" t="n">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="H363" t="n">
-        <v>3.21</v>
+        <v>3.57</v>
       </c>
       <c r="I363" t="n">
-        <v>5.44</v>
+        <v>5.16</v>
       </c>
       <c r="J363" t="inlineStr"/>
       <c r="K363" t="inlineStr"/>
@@ -23603,27 +23603,27 @@
         <v>3</v>
       </c>
       <c r="M363" t="n">
-        <v>0.72</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="N363" t="inlineStr"/>
       <c r="O363" t="inlineStr">
         <is>
-          <t>{"Aaron": {"actual": 8.75, "available": 14.0}, "Bailey": {"actual": 0.0, "available": 0.0}, "Corie": {"actual": 14.58, "available": 17.0}, "Erin": {"actual": 0.0, "available": 0.0}, "Maddy": {"actual": 0.0, "available": 0.0}, "Morgan": {"actual": 0.0, "available": 0.0}, "Natalie": {"actual": 0.0, "available": 12.5}, "Raquel": {"actual": 0.0, "available": 0.0}, "Nate": {"actual": 3.5, "available": 10.0}, "Liam": {"actual": 0.0, "available": 0.0}, "Andrew": {"actual": 0.0, "available": 0.0}, "Ellen": {"actual": 0.0, "available": 0.0}, "Lisa": {"actual": 0.0, "available": 0.0}, "Sarah": {"actual": 0.0, "available": 0.0}, "Tou": {"actual": 0.0, "available": 0.0}}</t>
+          <t>{"Aaron": {"actual": 11.75, "available": 14.0}, "Bailey": {"actual": 0.0, "available": 0.0}, "Corie": {"actual": 14.58, "available": 17.0}, "Erin": {"actual": 0.0, "available": 0.0}, "Maddy": {"actual": 0.0, "available": 0.0}, "Morgan": {"actual": 0.0, "available": 0.0}, "Natalie": {"actual": 0.0, "available": 12.5}, "Raquel": {"actual": 0.0, "available": 0.0}, "Nate": {"actual": 3.5, "available": 10.0}, "Liam": {"actual": 0.0, "available": 0.0}, "Andrew": {"actual": 0.0, "available": 0.0}, "Ellen": {"actual": 0.0, "available": 0.0}, "Lisa": {"actual": 0.0, "available": 0.0}, "Sarah": {"actual": 0.0, "available": 0.0}, "Tou": {"actual": 0.0, "available": 0.0}}</t>
         </is>
       </c>
       <c r="P363" t="inlineStr">
         <is>
-          <t>{"Aaron": {"output": 57.0, "target": 58.67}, "Corie": {"output": 35.0, "target": 45.83}, "Natalie": {"output": 0.0, "target": 0.0}, "Nate": {"output": 35.0, "target": 35.0}}</t>
+          <t>{"Aaron": {"output": 65.0, "target": 74.67}, "Corie": {"output": 35.0, "target": 45.83}, "Natalie": {"output": 1.0, "target": 0.0}, "Nate": {"output": 35.0, "target": 35.0}}</t>
         </is>
       </c>
       <c r="Q363" t="inlineStr">
         <is>
-          <t>{"Closures": {"output": 8.0, "target": 14.0}, "Inbox": {"output": 32.0, "target": 20.83}, "KO (Kick Outs)": {"output": 5.0, "target": 3.0}, "New Information": {"output": 28.0, "target": 39.0}, "Pending RD's": {"output": 11.0, "target": 16.0}, "SR's (Staging Records)": {"output": 43.0, "target": 46.67}}</t>
+          <t>{"Closures": {"output": 8.0, "target": 14.0}, "Inbox": {"output": 32.0, "target": 20.83}, "KO (Kick Outs)": {"output": 5.0, "target": 3.0}, "New Information": {"output": 29.0, "target": 39.0}, "Pending RD's": {"output": 14.0, "target": 22.0}, "SR's (Staging Records)": {"output": 48.0, "target": 56.67}}</t>
         </is>
       </c>
       <c r="R363" t="inlineStr">
         <is>
-          <t>{"Closures": 2.0, "Inbox": 2.08, "KO (Kick Outs)": 3.0, "New Information": 9.75, "Pending RD's": 5.33, "SR's (Staging Records)": 4.67}</t>
+          <t>{"Closures": 2.0, "Inbox": 2.08, "KO (Kick Outs)": 3.0, "New Information": 9.75, "Pending RD's": 7.33, "SR's (Staging Records)": 5.67}</t>
         </is>
       </c>
       <c r="S363" t="n">

</xml_diff>

<commit_message>
TCT Comm is good
</commit_message>
<xml_diff>
--- a/metrics_aggregate_dev.xlsx
+++ b/metrics_aggregate_dev.xlsx
@@ -25060,16 +25060,16 @@
         <v>82.91666666666667</v>
       </c>
       <c r="F385" t="n">
-        <v>317.3333333333333</v>
+        <v>324.3333333333333</v>
       </c>
       <c r="G385" t="n">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="H385" t="n">
-        <v>2</v>
+        <v>2.04</v>
       </c>
       <c r="I385" t="n">
-        <v>3.74</v>
+        <v>3.82</v>
       </c>
       <c r="J385" t="inlineStr"/>
       <c r="K385" t="inlineStr"/>
@@ -25082,22 +25082,22 @@
       <c r="N385" t="inlineStr"/>
       <c r="O385" t="inlineStr">
         <is>
-          <t>{"Aaron": {"actual": 0.0, "available": 0.0}, "Bailey": {"actual": 0.0, "available": 0.0}, "Corie": {"actual": 0.0, "available": 0.0}, "Erin": {"actual": 12.0, "available": 12.0}, "Maddy": {"actual": 3.67, "available": 6.0}, "Morgan": {"actual": 12.0, "available": 30.0}, "Natalie": {"actual": 0.0, "available": 0.0}, "Raquel": {"actual": 12.0, "available": 29.0}, "Nate": {"actual": 4.0, "available": 10.0}, "Liam": {"actual": 3.75, "available": 10.0}, "Andrew": {"actual": 11.0, "available": 8.0}, "Ellen": {"actual": 0.0, "available": 0.0}, "Lisa": {"actual": 6.0, "available": 8.0}, "Sarah": {"actual": 12.0, "available": 17.0}, "Tou": {"actual": 12.0, "available": 29.0}}</t>
+          <t>{"Aaron": {"actual": 0.0, "available": 0.0}, "Bailey": {"actual": 0.0, "available": 0.0}, "Corie": {"actual": 0.0, "available": 0.0}, "Erin": {"actual": 12.0, "available": 12.0}, "Maddy": {"actual": 3.67, "available": 6.0}, "Morgan": {"actual": 14.0, "available": 30.0}, "Natalie": {"actual": 0.0, "available": 0.0}, "Raquel": {"actual": 12.0, "available": 29.0}, "Nate": {"actual": 4.0, "available": 10.0}, "Liam": {"actual": 4.25, "available": 10.0}, "Andrew": {"actual": 11.0, "available": 8.0}, "Ellen": {"actual": 0.0, "available": 0.0}, "Lisa": {"actual": 8.0, "available": 8.0}, "Sarah": {"actual": 12.0, "available": 17.0}, "Tou": {"actual": 12.0, "available": 29.0}}</t>
         </is>
       </c>
       <c r="P385" t="inlineStr">
         <is>
-          <t>{"Andrew": {"output": 6.0, "target": 18.5}, "Erin": {"output": 29.0, "target": 34.0}, "Liam": {"output": 40.0, "target": 37.5}, "Lisa": {"output": 2.0, "target": 6.0}, "Maddy": {"output": 11.0, "target": 10.33}, "Morgan": {"output": 35.0, "target": 36.0}, "Nate": {"output": 25.0, "target": 28.0}, "Raquel": {"output": 41.0, "target": 35.0}, "Sarah": {"output": 44.0, "target": 40.0}, "Tou": {"output": 77.0, "target": 72.0}}</t>
+          <t>{"Andrew": {"output": 6.0, "target": 18.5}, "Erin": {"output": 29.0, "target": 34.0}, "Liam": {"output": 41.0, "target": 38.5}, "Lisa": {"output": 4.0, "target": 8.0}, "Maddy": {"output": 11.0, "target": 10.33}, "Morgan": {"output": 39.0, "target": 40.0}, "Nate": {"output": 25.0, "target": 28.0}, "Raquel": {"output": 41.0, "target": 35.0}, "Sarah": {"output": 44.0, "target": 40.0}, "Tou": {"output": 77.0, "target": 72.0}}</t>
         </is>
       </c>
       <c r="Q385" t="inlineStr">
         <is>
-          <t>{"Analysis Letters": {"output": 2.0, "target": 4.0}, "Closures": {"output": 77.0, "target": 72.0}, "GFE -Email": {"output": 60.0, "target": 60.0}, "GFE -Fax /Phone call": {"output": 5.0, "target": 5.5}, "Inbox": {"output": 17.0, "target": 13.0}, "KO (Kick Outs)": {"output": 3.0, "target": 2.0}, "New Information": {"output": 84.0, "target": 84.0}, "Nurse Consult": {"output": 0.0, "target": 0.0}, "Pending RD's": {"output": 26.0, "target": 23.33}, "RI's": {"output": 0.0, "target": 8.5}, "Reassess RD": {"output": 0.0, "target": 0.0}, "Registry": {"output": 0.0, "target": 2.0}, "Regulatory Reports Medwatch": {"output": 6.0, "target": 7.0}, "Regulatory Reports Vigilance": {"output": 8.0, "target": 8.0}, "SR's (Staging Records)": {"output": 22.0, "target": 28.0}}</t>
+          <t>{"Analysis Letters": {"output": 4.0, "target": 6.0}, "Closures": {"output": 77.0, "target": 72.0}, "GFE -Email": {"output": 60.0, "target": 60.0}, "GFE -Fax /Phone call": {"output": 6.0, "target": 6.5}, "Inbox": {"output": 17.0, "target": 13.0}, "KO (Kick Outs)": {"output": 3.0, "target": 2.0}, "New Information": {"output": 84.0, "target": 84.0}, "Nurse Consult": {"output": 0.0, "target": 0.0}, "Pending RD's": {"output": 26.0, "target": 23.33}, "RI's": {"output": 0.0, "target": 8.5}, "Reassess RD": {"output": 0.0, "target": 0.0}, "Registry": {"output": 0.0, "target": 2.0}, "Regulatory Reports Medwatch": {"output": 6.0, "target": 7.0}, "Regulatory Reports Vigilance": {"output": 8.0, "target": 8.0}, "SR's (Staging Records)": {"output": 26.0, "target": 32.0}}</t>
         </is>
       </c>
       <c r="R385" t="inlineStr">
         <is>
-          <t>{"Analysis Letters": 4.0, "Closures": 9.0, "GFE -Email": 5.0, "GFE -Fax /Phone call": 2.75, "Inbox": 1.0, "KO (Kick Outs)": 2.0, "New Information": 21.0, "Pending RD's": 11.67, "RI's": 8.5, "Registry": 2.0, "Regulatory Reports Medwatch": 3.5, "Regulatory Reports Vigilance": 4.0, "SR's (Staging Records)": 14.0}</t>
+          <t>{"Analysis Letters": 6.0, "Closures": 9.0, "GFE -Email": 5.0, "GFE -Fax /Phone call": 3.25, "Inbox": 1.0, "KO (Kick Outs)": 2.0, "New Information": 21.0, "Pending RD's": 11.67, "RI's": 8.5, "Registry": 2.0, "Regulatory Reports Medwatch": 3.5, "Regulatory Reports Vigilance": 4.0, "SR's (Staging Records)": 16.0}</t>
         </is>
       </c>
       <c r="S385" t="n">

</xml_diff>

<commit_message>
Added OCT to CAS
</commit_message>
<xml_diff>
--- a/metrics_aggregate_dev.xlsx
+++ b/metrics_aggregate_dev.xlsx
@@ -2343,7 +2343,9 @@
         </is>
       </c>
       <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
+      <c r="S28" t="n">
+        <v>93</v>
+      </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
     </row>
@@ -2404,7 +2406,9 @@
         </is>
       </c>
       <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
+      <c r="S29" t="n">
+        <v>93</v>
+      </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
     </row>
@@ -2465,7 +2469,9 @@
         </is>
       </c>
       <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
+      <c r="S30" t="n">
+        <v>93</v>
+      </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
     </row>
@@ -2526,7 +2532,9 @@
         </is>
       </c>
       <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
+      <c r="S31" t="n">
+        <v>93</v>
+      </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
     </row>
@@ -2587,7 +2595,9 @@
         </is>
       </c>
       <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
+      <c r="S32" t="n">
+        <v>93</v>
+      </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
     </row>
@@ -2648,7 +2658,9 @@
         </is>
       </c>
       <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
+      <c r="S33" t="n">
+        <v>93</v>
+      </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
     </row>
@@ -2709,7 +2721,9 @@
         </is>
       </c>
       <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
+      <c r="S34" t="n">
+        <v>93</v>
+      </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
     </row>
@@ -2770,7 +2784,9 @@
         </is>
       </c>
       <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
+      <c r="S35" t="n">
+        <v>93</v>
+      </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
     </row>
@@ -2831,7 +2847,9 @@
         </is>
       </c>
       <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
+      <c r="S36" t="n">
+        <v>93</v>
+      </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
     </row>
@@ -2892,7 +2910,9 @@
         </is>
       </c>
       <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
+      <c r="S37" t="n">
+        <v>92</v>
+      </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
     </row>
@@ -2953,7 +2973,9 @@
         </is>
       </c>
       <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
+      <c r="S38" t="n">
+        <v>92</v>
+      </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
     </row>
@@ -3014,7 +3036,9 @@
         </is>
       </c>
       <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
+      <c r="S39" t="n">
+        <v>92</v>
+      </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
     </row>
@@ -3075,7 +3099,9 @@
         </is>
       </c>
       <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
+      <c r="S40" t="n">
+        <v>92</v>
+      </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
     </row>
@@ -3136,7 +3162,9 @@
         </is>
       </c>
       <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
+      <c r="S41" t="n">
+        <v>94</v>
+      </c>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
     </row>
@@ -3197,7 +3225,9 @@
         </is>
       </c>
       <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
+      <c r="S42" t="n">
+        <v>94</v>
+      </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
     </row>
@@ -3258,7 +3288,9 @@
         </is>
       </c>
       <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
+      <c r="S43" t="n">
+        <v>94</v>
+      </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
     </row>
@@ -3319,7 +3351,9 @@
         </is>
       </c>
       <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
+      <c r="S44" t="n">
+        <v>94</v>
+      </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
     </row>
@@ -3380,7 +3414,9 @@
         </is>
       </c>
       <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
+      <c r="S45" t="n">
+        <v>94</v>
+      </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
     </row>
@@ -3441,7 +3477,9 @@
         </is>
       </c>
       <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
+      <c r="S46" t="n">
+        <v>92</v>
+      </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
     </row>
@@ -3502,7 +3540,9 @@
         </is>
       </c>
       <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
+      <c r="S47" t="n">
+        <v>92</v>
+      </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
     </row>
@@ -3563,7 +3603,9 @@
         </is>
       </c>
       <c r="R48" t="inlineStr"/>
-      <c r="S48" t="inlineStr"/>
+      <c r="S48" t="n">
+        <v>92</v>
+      </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
     </row>
@@ -3624,7 +3666,9 @@
         </is>
       </c>
       <c r="R49" t="inlineStr"/>
-      <c r="S49" t="inlineStr"/>
+      <c r="S49" t="n">
+        <v>92</v>
+      </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
     </row>
@@ -3685,7 +3729,9 @@
         </is>
       </c>
       <c r="R50" t="inlineStr"/>
-      <c r="S50" t="inlineStr"/>
+      <c r="S50" t="n">
+        <v>89</v>
+      </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
     </row>
@@ -3746,7 +3792,9 @@
         </is>
       </c>
       <c r="R51" t="inlineStr"/>
-      <c r="S51" t="inlineStr"/>
+      <c r="S51" t="n">
+        <v>89</v>
+      </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
     </row>
@@ -3807,7 +3855,9 @@
         </is>
       </c>
       <c r="R52" t="inlineStr"/>
-      <c r="S52" t="inlineStr"/>
+      <c r="S52" t="n">
+        <v>89</v>
+      </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
     </row>
@@ -3868,7 +3918,9 @@
         </is>
       </c>
       <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
+      <c r="S53" t="n">
+        <v>89</v>
+      </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
     </row>
@@ -3929,7 +3981,9 @@
         </is>
       </c>
       <c r="R54" t="inlineStr"/>
-      <c r="S54" t="inlineStr"/>
+      <c r="S54" t="n">
+        <v>90</v>
+      </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
     </row>
@@ -3990,7 +4044,9 @@
         </is>
       </c>
       <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr"/>
+      <c r="S55" t="n">
+        <v>90</v>
+      </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
     </row>
@@ -4051,7 +4107,9 @@
         </is>
       </c>
       <c r="R56" t="inlineStr"/>
-      <c r="S56" t="inlineStr"/>
+      <c r="S56" t="n">
+        <v>90</v>
+      </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
     </row>
@@ -4112,7 +4170,9 @@
         </is>
       </c>
       <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr"/>
+      <c r="S57" t="n">
+        <v>90</v>
+      </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
     </row>
@@ -4173,7 +4233,9 @@
         </is>
       </c>
       <c r="R58" t="inlineStr"/>
-      <c r="S58" t="inlineStr"/>
+      <c r="S58" t="n">
+        <v>90</v>
+      </c>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
     </row>
@@ -4234,7 +4296,9 @@
         </is>
       </c>
       <c r="R59" t="inlineStr"/>
-      <c r="S59" t="inlineStr"/>
+      <c r="S59" t="n">
+        <v>91</v>
+      </c>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
     </row>
@@ -4295,7 +4359,9 @@
         </is>
       </c>
       <c r="R60" t="inlineStr"/>
-      <c r="S60" t="inlineStr"/>
+      <c r="S60" t="n">
+        <v>91</v>
+      </c>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
     </row>
@@ -4356,7 +4422,9 @@
         </is>
       </c>
       <c r="R61" t="inlineStr"/>
-      <c r="S61" t="inlineStr"/>
+      <c r="S61" t="n">
+        <v>91</v>
+      </c>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
     </row>
@@ -4417,7 +4485,9 @@
         </is>
       </c>
       <c r="R62" t="inlineStr"/>
-      <c r="S62" t="inlineStr"/>
+      <c r="S62" t="n">
+        <v>91</v>
+      </c>
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr"/>
     </row>
@@ -4478,7 +4548,9 @@
         </is>
       </c>
       <c r="R63" t="inlineStr"/>
-      <c r="S63" t="inlineStr"/>
+      <c r="S63" t="n">
+        <v>87</v>
+      </c>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
     </row>
@@ -4539,7 +4611,9 @@
         </is>
       </c>
       <c r="R64" t="inlineStr"/>
-      <c r="S64" t="inlineStr"/>
+      <c r="S64" t="n">
+        <v>87</v>
+      </c>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
     </row>
@@ -4600,7 +4674,9 @@
         </is>
       </c>
       <c r="R65" t="inlineStr"/>
-      <c r="S65" t="inlineStr"/>
+      <c r="S65" t="n">
+        <v>87</v>
+      </c>
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
     </row>
@@ -4661,7 +4737,9 @@
         </is>
       </c>
       <c r="R66" t="inlineStr"/>
-      <c r="S66" t="inlineStr"/>
+      <c r="S66" t="n">
+        <v>87</v>
+      </c>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
     </row>
@@ -4722,7 +4800,9 @@
         </is>
       </c>
       <c r="R67" t="inlineStr"/>
-      <c r="S67" t="inlineStr"/>
+      <c r="S67" t="n">
+        <v>87</v>
+      </c>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
     </row>
@@ -4783,7 +4863,9 @@
         </is>
       </c>
       <c r="R68" t="inlineStr"/>
-      <c r="S68" t="inlineStr"/>
+      <c r="S68" t="n">
+        <v>92</v>
+      </c>
       <c r="T68" t="inlineStr"/>
       <c r="U68" t="inlineStr"/>
     </row>
@@ -4844,7 +4926,9 @@
         </is>
       </c>
       <c r="R69" t="inlineStr"/>
-      <c r="S69" t="inlineStr"/>
+      <c r="S69" t="n">
+        <v>92</v>
+      </c>
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
     </row>
@@ -4905,7 +4989,9 @@
         </is>
       </c>
       <c r="R70" t="inlineStr"/>
-      <c r="S70" t="inlineStr"/>
+      <c r="S70" t="n">
+        <v>92</v>
+      </c>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
     </row>
@@ -4966,7 +5052,9 @@
         </is>
       </c>
       <c r="R71" t="inlineStr"/>
-      <c r="S71" t="inlineStr"/>
+      <c r="S71" t="n">
+        <v>92</v>
+      </c>
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
     </row>
@@ -5027,7 +5115,9 @@
         </is>
       </c>
       <c r="R72" t="inlineStr"/>
-      <c r="S72" t="inlineStr"/>
+      <c r="S72" t="n">
+        <v>90</v>
+      </c>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
     </row>
@@ -5088,7 +5178,9 @@
         </is>
       </c>
       <c r="R73" t="inlineStr"/>
-      <c r="S73" t="inlineStr"/>
+      <c r="S73" t="n">
+        <v>90</v>
+      </c>
       <c r="T73" t="inlineStr"/>
       <c r="U73" t="inlineStr"/>
     </row>
@@ -5149,7 +5241,9 @@
         </is>
       </c>
       <c r="R74" t="inlineStr"/>
-      <c r="S74" t="inlineStr"/>
+      <c r="S74" t="n">
+        <v>90</v>
+      </c>
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
     </row>
@@ -5210,7 +5304,9 @@
         </is>
       </c>
       <c r="R75" t="inlineStr"/>
-      <c r="S75" t="inlineStr"/>
+      <c r="S75" t="n">
+        <v>90</v>
+      </c>
       <c r="T75" t="inlineStr"/>
       <c r="U75" t="inlineStr"/>
     </row>
@@ -5271,7 +5367,9 @@
         </is>
       </c>
       <c r="R76" t="inlineStr"/>
-      <c r="S76" t="inlineStr"/>
+      <c r="S76" t="n">
+        <v>88</v>
+      </c>
       <c r="T76" t="inlineStr"/>
       <c r="U76" t="inlineStr"/>
     </row>
@@ -5332,7 +5430,9 @@
         </is>
       </c>
       <c r="R77" t="inlineStr"/>
-      <c r="S77" t="inlineStr"/>
+      <c r="S77" t="n">
+        <v>88</v>
+      </c>
       <c r="T77" t="inlineStr"/>
       <c r="U77" t="inlineStr"/>
     </row>
@@ -5393,7 +5493,9 @@
         </is>
       </c>
       <c r="R78" t="inlineStr"/>
-      <c r="S78" t="inlineStr"/>
+      <c r="S78" t="n">
+        <v>88</v>
+      </c>
       <c r="T78" t="inlineStr"/>
       <c r="U78" t="inlineStr"/>
     </row>
@@ -5452,7 +5554,9 @@
         </is>
       </c>
       <c r="R79" t="inlineStr"/>
-      <c r="S79" t="inlineStr"/>
+      <c r="S79" t="n">
+        <v>88</v>
+      </c>
       <c r="T79" t="inlineStr"/>
       <c r="U79" t="inlineStr"/>
     </row>
@@ -5513,7 +5617,9 @@
         </is>
       </c>
       <c r="R80" t="inlineStr"/>
-      <c r="S80" t="inlineStr"/>
+      <c r="S80" t="n">
+        <v>88</v>
+      </c>
       <c r="T80" t="inlineStr"/>
       <c r="U80" t="inlineStr"/>
     </row>
@@ -5574,7 +5680,9 @@
         </is>
       </c>
       <c r="R81" t="inlineStr"/>
-      <c r="S81" t="inlineStr"/>
+      <c r="S81" t="n">
+        <v>88</v>
+      </c>
       <c r="T81" t="inlineStr"/>
       <c r="U81" t="inlineStr"/>
     </row>
@@ -5635,7 +5743,9 @@
         </is>
       </c>
       <c r="R82" t="inlineStr"/>
-      <c r="S82" t="inlineStr"/>
+      <c r="S82" t="n">
+        <v>88</v>
+      </c>
       <c r="T82" t="inlineStr"/>
       <c r="U82" t="inlineStr"/>
     </row>
@@ -5696,7 +5806,9 @@
         </is>
       </c>
       <c r="R83" t="inlineStr"/>
-      <c r="S83" t="inlineStr"/>
+      <c r="S83" t="n">
+        <v>88</v>
+      </c>
       <c r="T83" t="inlineStr"/>
       <c r="U83" t="inlineStr"/>
     </row>
@@ -5757,7 +5869,9 @@
         </is>
       </c>
       <c r="R84" t="inlineStr"/>
-      <c r="S84" t="inlineStr"/>
+      <c r="S84" t="n">
+        <v>88</v>
+      </c>
       <c r="T84" t="inlineStr"/>
       <c r="U84" t="inlineStr"/>
     </row>
@@ -5818,7 +5932,9 @@
         </is>
       </c>
       <c r="R85" t="inlineStr"/>
-      <c r="S85" t="inlineStr"/>
+      <c r="S85" t="n">
+        <v>83</v>
+      </c>
       <c r="T85" t="inlineStr"/>
       <c r="U85" t="inlineStr"/>
     </row>
@@ -5879,7 +5995,9 @@
         </is>
       </c>
       <c r="R86" t="inlineStr"/>
-      <c r="S86" t="inlineStr"/>
+      <c r="S86" t="n">
+        <v>83</v>
+      </c>
       <c r="T86" t="inlineStr"/>
       <c r="U86" t="inlineStr"/>
     </row>
@@ -5940,7 +6058,9 @@
         </is>
       </c>
       <c r="R87" t="inlineStr"/>
-      <c r="S87" t="inlineStr"/>
+      <c r="S87" t="n">
+        <v>83</v>
+      </c>
       <c r="T87" t="inlineStr"/>
       <c r="U87" t="inlineStr"/>
     </row>
@@ -6001,7 +6121,9 @@
         </is>
       </c>
       <c r="R88" t="inlineStr"/>
-      <c r="S88" t="inlineStr"/>
+      <c r="S88" t="n">
+        <v>83</v>
+      </c>
       <c r="T88" t="inlineStr"/>
       <c r="U88" t="inlineStr"/>
     </row>
@@ -6062,7 +6184,9 @@
         </is>
       </c>
       <c r="R89" t="inlineStr"/>
-      <c r="S89" t="inlineStr"/>
+      <c r="S89" t="n">
+        <v>86</v>
+      </c>
       <c r="T89" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
     </row>
@@ -6123,7 +6247,9 @@
         </is>
       </c>
       <c r="R90" t="inlineStr"/>
-      <c r="S90" t="inlineStr"/>
+      <c r="S90" t="n">
+        <v>86</v>
+      </c>
       <c r="T90" t="inlineStr"/>
       <c r="U90" t="inlineStr"/>
     </row>
@@ -6184,7 +6310,9 @@
         </is>
       </c>
       <c r="R91" t="inlineStr"/>
-      <c r="S91" t="inlineStr"/>
+      <c r="S91" t="n">
+        <v>86</v>
+      </c>
       <c r="T91" t="inlineStr"/>
       <c r="U91" t="inlineStr"/>
     </row>
@@ -6245,7 +6373,9 @@
         </is>
       </c>
       <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
+      <c r="S92" t="n">
+        <v>86</v>
+      </c>
       <c r="T92" t="inlineStr"/>
       <c r="U92" t="inlineStr"/>
     </row>
@@ -6306,7 +6436,9 @@
         </is>
       </c>
       <c r="R93" t="inlineStr"/>
-      <c r="S93" t="inlineStr"/>
+      <c r="S93" t="n">
+        <v>86</v>
+      </c>
       <c r="T93" t="inlineStr"/>
       <c r="U93" t="inlineStr"/>
     </row>
@@ -6367,7 +6499,9 @@
         </is>
       </c>
       <c r="R94" t="inlineStr"/>
-      <c r="S94" t="inlineStr"/>
+      <c r="S94" t="n">
+        <v>88</v>
+      </c>
       <c r="T94" t="inlineStr"/>
       <c r="U94" t="inlineStr"/>
     </row>
@@ -6428,7 +6562,9 @@
         </is>
       </c>
       <c r="R95" t="inlineStr"/>
-      <c r="S95" t="inlineStr"/>
+      <c r="S95" t="n">
+        <v>88</v>
+      </c>
       <c r="T95" t="inlineStr"/>
       <c r="U95" t="inlineStr"/>
     </row>
@@ -6489,7 +6625,9 @@
         </is>
       </c>
       <c r="R96" t="inlineStr"/>
-      <c r="S96" t="inlineStr"/>
+      <c r="S96" t="n">
+        <v>88</v>
+      </c>
       <c r="T96" t="inlineStr"/>
       <c r="U96" t="inlineStr"/>
     </row>
@@ -6550,7 +6688,9 @@
         </is>
       </c>
       <c r="R97" t="inlineStr"/>
-      <c r="S97" t="inlineStr"/>
+      <c r="S97" t="n">
+        <v>88</v>
+      </c>
       <c r="T97" t="inlineStr"/>
       <c r="U97" t="inlineStr"/>
     </row>
@@ -6611,7 +6751,9 @@
         </is>
       </c>
       <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
+      <c r="S98" t="n">
+        <v>88</v>
+      </c>
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
     </row>
@@ -6672,7 +6814,9 @@
         </is>
       </c>
       <c r="R99" t="inlineStr"/>
-      <c r="S99" t="inlineStr"/>
+      <c r="S99" t="n">
+        <v>88</v>
+      </c>
       <c r="T99" t="inlineStr"/>
       <c r="U99" t="inlineStr"/>
     </row>
@@ -6733,7 +6877,9 @@
         </is>
       </c>
       <c r="R100" t="inlineStr"/>
-      <c r="S100" t="inlineStr"/>
+      <c r="S100" t="n">
+        <v>88</v>
+      </c>
       <c r="T100" t="inlineStr"/>
       <c r="U100" t="inlineStr"/>
     </row>
@@ -6794,7 +6940,9 @@
         </is>
       </c>
       <c r="R101" t="inlineStr"/>
-      <c r="S101" t="inlineStr"/>
+      <c r="S101" t="n">
+        <v>88</v>
+      </c>
       <c r="T101" t="inlineStr"/>
       <c r="U101" t="inlineStr"/>
     </row>
@@ -6855,7 +7003,9 @@
         </is>
       </c>
       <c r="R102" t="inlineStr"/>
-      <c r="S102" t="inlineStr"/>
+      <c r="S102" t="n">
+        <v>89</v>
+      </c>
       <c r="T102" t="inlineStr"/>
       <c r="U102" t="inlineStr"/>
     </row>
@@ -6916,7 +7066,9 @@
         </is>
       </c>
       <c r="R103" t="inlineStr"/>
-      <c r="S103" t="inlineStr"/>
+      <c r="S103" t="n">
+        <v>89</v>
+      </c>
       <c r="T103" t="inlineStr"/>
       <c r="U103" t="inlineStr"/>
     </row>
@@ -6977,7 +7129,9 @@
         </is>
       </c>
       <c r="R104" t="inlineStr"/>
-      <c r="S104" t="inlineStr"/>
+      <c r="S104" t="n">
+        <v>89</v>
+      </c>
       <c r="T104" t="inlineStr"/>
       <c r="U104" t="inlineStr"/>
     </row>
@@ -7038,7 +7192,9 @@
         </is>
       </c>
       <c r="R105" t="inlineStr"/>
-      <c r="S105" t="inlineStr"/>
+      <c r="S105" t="n">
+        <v>89</v>
+      </c>
       <c r="T105" t="inlineStr"/>
       <c r="U105" t="inlineStr"/>
     </row>
@@ -7099,7 +7255,9 @@
         </is>
       </c>
       <c r="R106" t="inlineStr"/>
-      <c r="S106" t="inlineStr"/>
+      <c r="S106" t="n">
+        <v>87</v>
+      </c>
       <c r="T106" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
     </row>
@@ -7160,7 +7318,9 @@
         </is>
       </c>
       <c r="R107" t="inlineStr"/>
-      <c r="S107" t="inlineStr"/>
+      <c r="S107" t="n">
+        <v>87</v>
+      </c>
       <c r="T107" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
     </row>
@@ -7221,7 +7381,9 @@
         </is>
       </c>
       <c r="R108" t="inlineStr"/>
-      <c r="S108" t="inlineStr"/>
+      <c r="S108" t="n">
+        <v>88</v>
+      </c>
       <c r="T108" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
     </row>
@@ -7282,7 +7444,9 @@
         </is>
       </c>
       <c r="R109" t="inlineStr"/>
-      <c r="S109" t="inlineStr"/>
+      <c r="S109" t="n">
+        <v>88</v>
+      </c>
       <c r="T109" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
     </row>
@@ -7343,7 +7507,9 @@
         </is>
       </c>
       <c r="R110" t="inlineStr"/>
-      <c r="S110" t="inlineStr"/>
+      <c r="S110" t="n">
+        <v>87</v>
+      </c>
       <c r="T110" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
     </row>
@@ -7404,7 +7570,9 @@
         </is>
       </c>
       <c r="R111" t="inlineStr"/>
-      <c r="S111" t="inlineStr"/>
+      <c r="S111" t="n">
+        <v>88</v>
+      </c>
       <c r="T111" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
     </row>
@@ -7465,7 +7633,9 @@
         </is>
       </c>
       <c r="R112" t="inlineStr"/>
-      <c r="S112" t="inlineStr"/>
+      <c r="S112" t="n">
+        <v>87</v>
+      </c>
       <c r="T112" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
     </row>
@@ -7526,7 +7696,9 @@
         </is>
       </c>
       <c r="R113" t="inlineStr"/>
-      <c r="S113" t="inlineStr"/>
+      <c r="S113" t="n">
+        <v>86</v>
+      </c>
       <c r="T113" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
     </row>
@@ -7587,7 +7759,9 @@
         </is>
       </c>
       <c r="R114" t="inlineStr"/>
-      <c r="S114" t="inlineStr"/>
+      <c r="S114" t="n">
+        <v>86</v>
+      </c>
       <c r="T114" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
     </row>
@@ -7648,7 +7822,9 @@
         </is>
       </c>
       <c r="R115" t="inlineStr"/>
-      <c r="S115" t="inlineStr"/>
+      <c r="S115" t="n">
+        <v>86</v>
+      </c>
       <c r="T115" t="inlineStr"/>
       <c r="U115" t="inlineStr"/>
     </row>
@@ -7709,7 +7885,9 @@
         </is>
       </c>
       <c r="R116" t="inlineStr"/>
-      <c r="S116" t="inlineStr"/>
+      <c r="S116" t="n">
+        <v>86</v>
+      </c>
       <c r="T116" t="inlineStr"/>
       <c r="U116" t="inlineStr"/>
     </row>
@@ -7770,7 +7948,9 @@
         </is>
       </c>
       <c r="R117" t="inlineStr"/>
-      <c r="S117" t="inlineStr"/>
+      <c r="S117" t="n">
+        <v>85</v>
+      </c>
       <c r="T117" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
     </row>
@@ -7831,7 +8011,9 @@
         </is>
       </c>
       <c r="R118" t="inlineStr"/>
-      <c r="S118" t="inlineStr"/>
+      <c r="S118" t="n">
+        <v>87</v>
+      </c>
       <c r="T118" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
     </row>
@@ -7892,7 +8074,9 @@
         </is>
       </c>
       <c r="R119" t="inlineStr"/>
-      <c r="S119" t="inlineStr"/>
+      <c r="S119" t="n">
+        <v>87</v>
+      </c>
       <c r="T119" t="inlineStr"/>
       <c r="U119" t="inlineStr"/>
     </row>
@@ -7953,7 +8137,9 @@
         </is>
       </c>
       <c r="R120" t="inlineStr"/>
-      <c r="S120" t="inlineStr"/>
+      <c r="S120" t="n">
+        <v>87</v>
+      </c>
       <c r="T120" t="inlineStr"/>
       <c r="U120" t="inlineStr"/>
     </row>
@@ -7981,13 +8167,13 @@
         <v>850</v>
       </c>
       <c r="G121" t="n">
-        <v>617</v>
+        <v>671</v>
       </c>
       <c r="H121" t="n">
         <v>7.73</v>
       </c>
       <c r="I121" t="n">
-        <v>3.31</v>
+        <v>3.6</v>
       </c>
       <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
@@ -8005,16 +8191,18 @@
       </c>
       <c r="P121" t="inlineStr">
         <is>
-          <t>{"Alexa": {"output": 0.0, "target": 34.0}, "GMED CIT": {"output": 0.0, "target": 0.0}, "Gina": {"output": 28.0, "target": 20.0}, "Gina - Affera": {"output": 45.0, "target": 64.0}, "Gina, Golden, Ruth": {"output": 0.0, "target": 0.0}, "Golden": {"output": 80.0, "target": 98.0}, "Golden, Orla, Natalie": {"output": 0.0, "target": 0.0}, "Jerlie": {"output": 13.0, "target": 74.0}, "Jyn": {"output": 41.0, "target": 0.0}, "Lauren": {"output": 94.0, "target": 96.0}, "Marie": {"output": 44.0, "target": 50.0}, "Natalie": {"output": 67.0, "target": 66.0}, "Natalie and Ruth": {"output": 2.0, "target": 2.0}, "Orla": {"output": 52.0, "target": 68.0}, "Orla, Gina": {"output": 0.0, "target": 0.0}, "Ruth": {"output": 0.0, "target": 4.0}, "Ruth - Prism 2": {"output": 27.0, "target": 68.0}, "Ruth and Natalie": {"output": 2.0, "target": 4.0}, "Sai": {"output": 62.0, "target": 10.0}, "Sean": {"output": 60.0, "target": 78.0}, "Team Member": {"output": 0.0, "target": 0.0}, "nan": {"output": 0.0, "target": 114.0}}</t>
+          <t>{"Alexa": {"output": 0.0, "target": 34.0}, "GMED CIT": {"output": 0.0, "target": 0.0}, "Gina": {"output": 28.0, "target": 20.0}, "Gina - Affera": {"output": 45.0, "target": 64.0}, "Gina, Golden, Ruth": {"output": 0.0, "target": 0.0}, "Golden": {"output": 108.0, "target": 98.0}, "Golden, Orla, Natalie": {"output": 0.0, "target": 0.0}, "Jerlie": {"output": 13.0, "target": 74.0}, "Jyn": {"output": 41.0, "target": 0.0}, "Lauren": {"output": 94.0, "target": 96.0}, "Marie": {"output": 44.0, "target": 50.0}, "Natalie": {"output": 67.0, "target": 66.0}, "Natalie and Ruth": {"output": 2.0, "target": 2.0}, "Orla": {"output": 78.0, "target": 68.0}, "Orla, Gina": {"output": 0.0, "target": 0.0}, "Ruth": {"output": 0.0, "target": 4.0}, "Ruth - Prism 2": {"output": 27.0, "target": 68.0}, "Ruth and Natalie": {"output": 2.0, "target": 4.0}, "Sai": {"output": 62.0, "target": 10.0}, "Sean": {"output": 60.0, "target": 78.0}, "Team Member": {"output": 0.0, "target": 0.0}, "nan": {"output": 0.0, "target": 114.0}}</t>
         </is>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>{"Audit": {"output": 0.0, "target": 0.0}, "COS Pitches": {"output": 0.0, "target": 0.0}, "Comm (email rec'd, BUAR)": {"output": 116.0, "target": 192.0}, "Complaint Wizard SR to RD/RR": {"output": 132.0, "target": 216.0}, "Complaint Wizard SR to RD/RR -": {"output": 21.0, "target": 32.0}, "FAC - NON FER": {"output": 18.0, "target": 0.0}, "Inbox": {"output": 0.0, "target": 0.0}, "Letters": {"output": 4.0, "target": 54.0}, "Literature": {"output": 1.0, "target": 0.0}, "NC SR": {"output": 0.0, "target": 0.0}, "NextGen": {"output": 0.0, "target": 0.0}, "NextGen/Lates": {"output": 0.0, "target": 0.0}, "OOO": {"output": 0.0, "target": 0.0}, "Prism 1 - comm, tasks, reg reports": {"output": 0.0, "target": 0.0}, "Reassess INV tasks": {"output": 0.0, "target": 0.0}, "Regulatory Inquiries": {"output": 0.0, "target": 0.0}, "Station 2 (In progress, pending comm thru due date)": {"output": 72.0, "target": 70.0}, "Station 3 Reassess RD": {"output": 123.0, "target": 120.0}, "Station Work": {"output": 0.0, "target": 0.0}, "Tasks (EU &amp; US)": {"output": 0.0, "target": 6.0}, "Tasks (EU)": {"output": 42.0, "target": 66.0}, "Tasks (US &amp; EU)": {"output": 13.0, "target": 12.0}, "Tasks (US)": {"output": 41.0, "target": 42.0}, "Vig/US Supplemental RR": {"output": 34.0, "target": 40.0}, "Yellow Belt": {"output": 0.0, "target": 0.0}, "nan": {"output": 0.0, "target": 0.0}}</t>
+          <t>{"Audit": {"output": 0.0, "target": 0.0}, "COS Pitches": {"output": 0.0, "target": 0.0}, "Comm (email rec'd, BUAR)": {"output": 134.0, "target": 192.0}, "Complaint Wizard SR to RD/RR": {"output": 148.0, "target": 216.0}, "Complaint Wizard SR to RD/RR -": {"output": 21.0, "target": 32.0}, "FAC - NON FER": {"output": 18.0, "target": 0.0}, "Inbox": {"output": 0.0, "target": 0.0}, "Letters": {"output": 4.0, "target": 54.0}, "Literature": {"output": 1.0, "target": 0.0}, "NC SR": {"output": 0.0, "target": 0.0}, "NextGen": {"output": 0.0, "target": 0.0}, "NextGen/Lates": {"output": 0.0, "target": 0.0}, "OOO": {"output": 0.0, "target": 0.0}, "Prism 1 - comm, tasks, reg reports": {"output": 0.0, "target": 0.0}, "Reassess INV tasks": {"output": 0.0, "target": 0.0}, "Regulatory Inquiries": {"output": 0.0, "target": 0.0}, "Station 2 (In progress, pending comm thru due date)": {"output": 72.0, "target": 70.0}, "Station 3 Reassess RD": {"output": 123.0, "target": 120.0}, "Station Work": {"output": 0.0, "target": 0.0}, "Tasks (EU &amp; US)": {"output": 0.0, "target": 6.0}, "Tasks (EU)": {"output": 42.0, "target": 66.0}, "Tasks (US &amp; EU)": {"output": 13.0, "target": 12.0}, "Tasks (US)": {"output": 61.0, "target": 42.0}, "Vig/US Supplemental RR": {"output": 34.0, "target": 40.0}, "Yellow Belt": {"output": 0.0, "target": 0.0}, "nan": {"output": 0.0, "target": 0.0}}</t>
         </is>
       </c>
       <c r="R121" t="inlineStr"/>
-      <c r="S121" t="inlineStr"/>
+      <c r="S121" t="n">
+        <v>88</v>
+      </c>
       <c r="T121" t="inlineStr"/>
       <c r="U121" t="inlineStr"/>
     </row>

</xml_diff>